<commit_message>
updated HF for new avg periods
</commit_message>
<xml_diff>
--- a/GSD/baskets_new_sizes/basketGSD_hypflux_CS1mm.xlsx
+++ b/GSD/baskets_new_sizes/basketGSD_hypflux_CS1mm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\baskets_new_sizes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38774FF-B6E5-4410-9461-1D98B05CA901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34D5843-72C0-451A-B739-6AEC8DD8FA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FF2C68C4-0230-4397-BD30-01ABAA0FCBBF}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{FF2C68C4-0230-4397-BD30-01ABAA0FCBBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Spring Weights" sheetId="1" r:id="rId1"/>
@@ -2802,6 +2802,105 @@
     <xf numFmtId="2" fontId="3" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2820,108 +2919,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2940,19 +2940,19 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3984,31 +3984,31 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-0.20417995461623964</c:v>
+                  <c:v>-0.23784858917921259</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.20417995461623964</c:v>
+                  <c:v>-0.23784858917921259</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.31261653570633985</c:v>
+                  <c:v>-0.32194296104905268</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11724795870967698</c:v>
+                  <c:v>9.8870595823215071E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11724795870967698</c:v>
+                  <c:v>9.8870595823215071E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4.048383003337034E-2</c:v>
+                  <c:v>-5.1068450937348228E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.1076174245161288</c:v>
+                  <c:v>-0.12059113340456466</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.1076174245161288</c:v>
+                  <c:v>-0.12059113340456466</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-4.730072532146827E-2</c:v>
+                  <c:v>-5.0699230181641519E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4154,31 +4154,31 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-0.20417995461623964</c:v>
+                  <c:v>-0.23784858917921259</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.20417995461623964</c:v>
+                  <c:v>-0.23784858917921259</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.31261653570633985</c:v>
+                  <c:v>-0.32194296104905268</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11724795870967698</c:v>
+                  <c:v>9.8870595823215071E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11724795870967698</c:v>
+                  <c:v>9.8870595823215071E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4.048383003337034E-2</c:v>
+                  <c:v>-5.1068450937348228E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.1076174245161288</c:v>
+                  <c:v>-0.12059113340456466</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.1076174245161288</c:v>
+                  <c:v>-0.12059113340456466</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-4.730072532146827E-2</c:v>
+                  <c:v>-5.0699230181641519E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4324,31 +4324,31 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-0.20417995461623964</c:v>
+                  <c:v>-0.23784858917921259</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.20417995461623964</c:v>
+                  <c:v>-0.23784858917921259</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.31261653570633985</c:v>
+                  <c:v>-0.32194296104905268</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11724795870967698</c:v>
+                  <c:v>9.8870595823215071E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11724795870967698</c:v>
+                  <c:v>9.8870595823215071E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4.048383003337034E-2</c:v>
+                  <c:v>-5.1068450937348228E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.1076174245161288</c:v>
+                  <c:v>-0.12059113340456466</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.1076174245161288</c:v>
+                  <c:v>-0.12059113340456466</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-4.730072532146827E-2</c:v>
+                  <c:v>-5.0699230181641519E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4494,31 +4494,31 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-0.20417995461623964</c:v>
+                  <c:v>-0.23784858917921259</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.20417995461623964</c:v>
+                  <c:v>-0.23784858917921259</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.31261653570633985</c:v>
+                  <c:v>-0.32194296104905268</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11724795870967698</c:v>
+                  <c:v>9.8870595823215071E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11724795870967698</c:v>
+                  <c:v>9.8870595823215071E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4.048383003337034E-2</c:v>
+                  <c:v>-5.1068450937348228E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.1076174245161288</c:v>
+                  <c:v>-0.12059113340456466</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.1076174245161288</c:v>
+                  <c:v>-0.12059113340456466</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-4.730072532146827E-2</c:v>
+                  <c:v>-5.0699230181641519E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5109,28 +5109,28 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-0.20417995461623964</c:v>
+                  <c:v>-0.23784858917921259</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.31261653570633985</c:v>
+                  <c:v>-0.32194296104905268</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11724795870967698</c:v>
+                  <c:v>9.8870595823215071E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11724795870967698</c:v>
+                  <c:v>9.8870595823215071E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.048383003337034E-2</c:v>
+                  <c:v>-5.1068450937348228E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.1076174245161288</c:v>
+                  <c:v>-0.12059113340456466</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.1076174245161288</c:v>
+                  <c:v>-0.12059113340456466</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-4.730072532146827E-2</c:v>
+                  <c:v>-5.0699230181641519E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5273,28 +5273,28 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-0.20417995461623964</c:v>
+                  <c:v>-0.23784858917921259</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.31261653570633985</c:v>
+                  <c:v>-0.32194296104905268</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11724795870967698</c:v>
+                  <c:v>9.8870595823215071E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11724795870967698</c:v>
+                  <c:v>9.8870595823215071E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.048383003337034E-2</c:v>
+                  <c:v>-5.1068450937348228E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.1076174245161288</c:v>
+                  <c:v>-0.12059113340456466</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.1076174245161288</c:v>
+                  <c:v>-0.12059113340456466</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-4.730072532146827E-2</c:v>
+                  <c:v>-5.0699230181641519E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5438,28 +5438,28 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-0.20417995461623964</c:v>
+                  <c:v>-0.23784858917921259</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.31261653570633985</c:v>
+                  <c:v>-0.32194296104905268</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11724795870967698</c:v>
+                  <c:v>9.8870595823215071E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11724795870967698</c:v>
+                  <c:v>9.8870595823215071E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.048383003337034E-2</c:v>
+                  <c:v>-5.1068450937348228E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.1076174245161288</c:v>
+                  <c:v>-0.12059113340456466</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.1076174245161288</c:v>
+                  <c:v>-0.12059113340456466</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-4.730072532146827E-2</c:v>
+                  <c:v>-5.0699230181641519E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5602,28 +5602,28 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-0.20417995461623964</c:v>
+                  <c:v>-0.23784858917921259</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.31261653570633985</c:v>
+                  <c:v>-0.32194296104905268</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11724795870967698</c:v>
+                  <c:v>9.8870595823215071E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11724795870967698</c:v>
+                  <c:v>9.8870595823215071E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.048383003337034E-2</c:v>
+                  <c:v>-5.1068450937348228E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.1076174245161288</c:v>
+                  <c:v>-0.12059113340456466</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.1076174245161288</c:v>
+                  <c:v>-0.12059113340456466</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-4.730072532146827E-2</c:v>
+                  <c:v>-5.0699230181641519E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6247,37 +6247,37 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.22907037862867247</c:v>
+                  <c:v>0.20454360227175514</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22907037862867247</c:v>
+                  <c:v>0.20454360227175514</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.31502368370436307</c:v>
+                  <c:v>-0.31661374974045781</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-7.346940523597506E-2</c:v>
+                  <c:v>-0.11017208412824342</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.909818870881559E-2</c:v>
+                  <c:v>6.0405779541984679E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.909818870881559E-2</c:v>
+                  <c:v>6.0405779541984679E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.9825588886910034E-2</c:v>
+                  <c:v>-3.4732918409770948E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.9825588886910034E-2</c:v>
+                  <c:v>-3.4732918409770948E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.10258748751558326</c:v>
+                  <c:v>-0.16746416727938898</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.10258748751558326</c:v>
+                  <c:v>-0.16746416727938898</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-3.883410208370431E-2</c:v>
+                  <c:v>-3.3378369109007613E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6429,37 +6429,37 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.22907037862867247</c:v>
+                  <c:v>0.20454360227175514</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22907037862867247</c:v>
+                  <c:v>0.20454360227175514</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.31502368370436307</c:v>
+                  <c:v>-0.31661374974045781</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-7.346940523597506E-2</c:v>
+                  <c:v>-0.11017208412824342</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.909818870881559E-2</c:v>
+                  <c:v>6.0405779541984679E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.909818870881559E-2</c:v>
+                  <c:v>6.0405779541984679E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.9825588886910034E-2</c:v>
+                  <c:v>-3.4732918409770948E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.9825588886910034E-2</c:v>
+                  <c:v>-3.4732918409770948E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.10258748751558326</c:v>
+                  <c:v>-0.16746416727938898</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.10258748751558326</c:v>
+                  <c:v>-0.16746416727938898</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-3.883410208370431E-2</c:v>
+                  <c:v>-3.3378369109007613E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6611,37 +6611,37 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.22907037862867247</c:v>
+                  <c:v>0.20454360227175514</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22907037862867247</c:v>
+                  <c:v>0.20454360227175514</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.31502368370436307</c:v>
+                  <c:v>-0.31661374974045781</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-7.346940523597506E-2</c:v>
+                  <c:v>-0.11017208412824342</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.909818870881559E-2</c:v>
+                  <c:v>6.0405779541984679E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.909818870881559E-2</c:v>
+                  <c:v>6.0405779541984679E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.9825588886910034E-2</c:v>
+                  <c:v>-3.4732918409770948E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.9825588886910034E-2</c:v>
+                  <c:v>-3.4732918409770948E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.10258748751558326</c:v>
+                  <c:v>-0.16746416727938898</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.10258748751558326</c:v>
+                  <c:v>-0.16746416727938898</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-3.883410208370431E-2</c:v>
+                  <c:v>-3.3378369109007613E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6793,37 +6793,37 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.22907037862867247</c:v>
+                  <c:v>0.20454360227175514</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22907037862867247</c:v>
+                  <c:v>0.20454360227175514</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.31502368370436307</c:v>
+                  <c:v>-0.31661374974045781</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-7.346940523597506E-2</c:v>
+                  <c:v>-0.11017208412824342</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.909818870881559E-2</c:v>
+                  <c:v>6.0405779541984679E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.909818870881559E-2</c:v>
+                  <c:v>6.0405779541984679E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.9825588886910034E-2</c:v>
+                  <c:v>-3.4732918409770948E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.9825588886910034E-2</c:v>
+                  <c:v>-3.4732918409770948E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.10258748751558326</c:v>
+                  <c:v>-0.16746416727938898</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.10258748751558326</c:v>
+                  <c:v>-0.16746416727938898</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-3.883410208370431E-2</c:v>
+                  <c:v>-3.3378369109007613E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7460,31 +7460,31 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-0.21250269512953343</c:v>
+                  <c:v>-0.25646381521666273</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.21250269512953343</c:v>
+                  <c:v>-0.25646381521666273</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.31338709554404104</c:v>
+                  <c:v>-0.32648441197031308</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11558307282901517</c:v>
+                  <c:v>8.8871890830739209E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11558307282901517</c:v>
+                  <c:v>8.8871890830739209E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4.1403888746113962E-2</c:v>
+                  <c:v>-5.8003155872635853E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.10857605372020686</c:v>
+                  <c:v>-0.12379754395977956</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.10857605372020686</c:v>
+                  <c:v>-0.12379754395977956</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-4.7612346826943E-2</c:v>
+                  <c:v>-5.2460135362221633E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7630,31 +7630,31 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-0.21250269512953343</c:v>
+                  <c:v>-0.25646381521666273</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.21250269512953343</c:v>
+                  <c:v>-0.25646381521666273</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.31338709554404104</c:v>
+                  <c:v>-0.32648441197031308</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11558307282901517</c:v>
+                  <c:v>8.8871890830739209E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11558307282901517</c:v>
+                  <c:v>8.8871890830739209E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4.1403888746113962E-2</c:v>
+                  <c:v>-5.8003155872635853E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.10857605372020686</c:v>
+                  <c:v>-0.12379754395977956</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.10857605372020686</c:v>
+                  <c:v>-0.12379754395977956</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-4.7612346826943E-2</c:v>
+                  <c:v>-5.2460135362221633E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7800,31 +7800,31 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-0.21250269512953343</c:v>
+                  <c:v>-0.25646381521666273</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.21250269512953343</c:v>
+                  <c:v>-0.25646381521666273</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.31338709554404104</c:v>
+                  <c:v>-0.32648441197031308</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11558307282901517</c:v>
+                  <c:v>8.8871890830739209E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11558307282901517</c:v>
+                  <c:v>8.8871890830739209E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4.1403888746113962E-2</c:v>
+                  <c:v>-5.8003155872635853E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.10857605372020686</c:v>
+                  <c:v>-0.12379754395977956</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.10857605372020686</c:v>
+                  <c:v>-0.12379754395977956</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-4.7612346826943E-2</c:v>
+                  <c:v>-5.2460135362221633E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7970,31 +7970,31 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-0.21250269512953343</c:v>
+                  <c:v>-0.25646381521666273</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.21250269512953343</c:v>
+                  <c:v>-0.25646381521666273</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.31338709554404104</c:v>
+                  <c:v>-0.32648441197031308</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11558307282901517</c:v>
+                  <c:v>8.8871890830739209E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11558307282901517</c:v>
+                  <c:v>8.8871890830739209E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4.1403888746113962E-2</c:v>
+                  <c:v>-5.8003155872635853E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.10857605372020686</c:v>
+                  <c:v>-0.12379754395977956</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.10857605372020686</c:v>
+                  <c:v>-0.12379754395977956</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-4.7612346826943E-2</c:v>
+                  <c:v>-5.2460135362221633E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8585,28 +8585,28 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-0.21250269512953343</c:v>
+                  <c:v>-0.25646381521666273</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.31338709554404104</c:v>
+                  <c:v>-0.32648441197031308</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11558307282901517</c:v>
+                  <c:v>8.8871890830739209E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11558307282901517</c:v>
+                  <c:v>8.8871890830739209E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.1403888746113962E-2</c:v>
+                  <c:v>-5.8003155872635853E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.10857605372020686</c:v>
+                  <c:v>-0.12379754395977956</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.10857605372020686</c:v>
+                  <c:v>-0.12379754395977956</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-4.7612346826943E-2</c:v>
+                  <c:v>-5.2460135362221633E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8749,28 +8749,28 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-0.21250269512953343</c:v>
+                  <c:v>-0.25646381521666273</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.31338709554404104</c:v>
+                  <c:v>-0.32648441197031308</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11558307282901517</c:v>
+                  <c:v>8.8871890830739209E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11558307282901517</c:v>
+                  <c:v>8.8871890830739209E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.1403888746113962E-2</c:v>
+                  <c:v>-5.8003155872635853E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.10857605372020686</c:v>
+                  <c:v>-0.12379754395977956</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.10857605372020686</c:v>
+                  <c:v>-0.12379754395977956</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-4.7612346826943E-2</c:v>
+                  <c:v>-5.2460135362221633E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8914,28 +8914,28 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-0.21250269512953343</c:v>
+                  <c:v>-0.25646381521666273</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.31338709554404104</c:v>
+                  <c:v>-0.32648441197031308</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11558307282901517</c:v>
+                  <c:v>8.8871890830739209E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11558307282901517</c:v>
+                  <c:v>8.8871890830739209E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.1403888746113962E-2</c:v>
+                  <c:v>-5.8003155872635853E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.10857605372020686</c:v>
+                  <c:v>-0.12379754395977956</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.10857605372020686</c:v>
+                  <c:v>-0.12379754395977956</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-4.7612346826943E-2</c:v>
+                  <c:v>-5.2460135362221633E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9078,28 +9078,28 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-0.21250269512953343</c:v>
+                  <c:v>-0.25646381521666273</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.31338709554404104</c:v>
+                  <c:v>-0.32648441197031308</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11558307282901517</c:v>
+                  <c:v>8.8871890830739209E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11558307282901517</c:v>
+                  <c:v>8.8871890830739209E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.1403888746113962E-2</c:v>
+                  <c:v>-5.8003155872635853E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.10857605372020686</c:v>
+                  <c:v>-0.12379754395977956</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.10857605372020686</c:v>
+                  <c:v>-0.12379754395977956</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-4.7612346826943E-2</c:v>
+                  <c:v>-5.2460135362221633E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17697,37 +17697,37 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.18882498202240408</c:v>
+                  <c:v>0.20455321949518118</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18882498202240408</c:v>
+                  <c:v>0.20455321949518118</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.32061441221680753</c:v>
+                  <c:v>-0.31662176778338602</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.11450901614105548</c:v>
+                  <c:v>-0.11018080455254639</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.2373487372281072E-2</c:v>
+                  <c:v>6.039280873795317E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.2373487372281072E-2</c:v>
+                  <c:v>6.039280873795317E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.3609137631747582E-2</c:v>
+                  <c:v>-3.4741507318953639E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.3609137631747582E-2</c:v>
+                  <c:v>-3.4741507318953639E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.16211130541015681</c:v>
+                  <c:v>-0.16758290489215216</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.16211130541015681</c:v>
+                  <c:v>-0.16758290489215216</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-3.3646281336213321E-2</c:v>
+                  <c:v>-3.3385679140890294E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17879,37 +17879,37 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.18882498202240408</c:v>
+                  <c:v>0.20455321949518118</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18882498202240408</c:v>
+                  <c:v>0.20455321949518118</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.32061441221680753</c:v>
+                  <c:v>-0.31662176778338602</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.11450901614105548</c:v>
+                  <c:v>-0.11018080455254639</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.2373487372281072E-2</c:v>
+                  <c:v>6.039280873795317E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.2373487372281072E-2</c:v>
+                  <c:v>6.039280873795317E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.3609137631747582E-2</c:v>
+                  <c:v>-3.4741507318953639E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.3609137631747582E-2</c:v>
+                  <c:v>-3.4741507318953639E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.16211130541015681</c:v>
+                  <c:v>-0.16758290489215216</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.16211130541015681</c:v>
+                  <c:v>-0.16758290489215216</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-3.3646281336213321E-2</c:v>
+                  <c:v>-3.3385679140890294E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18061,37 +18061,37 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.18882498202240408</c:v>
+                  <c:v>0.20455321949518118</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18882498202240408</c:v>
+                  <c:v>0.20455321949518118</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.32061441221680753</c:v>
+                  <c:v>-0.31662176778338602</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.11450901614105548</c:v>
+                  <c:v>-0.11018080455254639</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.2373487372281072E-2</c:v>
+                  <c:v>6.039280873795317E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.2373487372281072E-2</c:v>
+                  <c:v>6.039280873795317E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.3609137631747582E-2</c:v>
+                  <c:v>-3.4741507318953639E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.3609137631747582E-2</c:v>
+                  <c:v>-3.4741507318953639E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.16211130541015681</c:v>
+                  <c:v>-0.16758290489215216</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.16211130541015681</c:v>
+                  <c:v>-0.16758290489215216</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-3.3646281336213321E-2</c:v>
+                  <c:v>-3.3385679140890294E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18243,37 +18243,37 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.18882498202240408</c:v>
+                  <c:v>0.20455321949518118</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18882498202240408</c:v>
+                  <c:v>0.20455321949518118</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.32061441221680753</c:v>
+                  <c:v>-0.31662176778338602</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.11450901614105548</c:v>
+                  <c:v>-0.11018080455254639</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.2373487372281072E-2</c:v>
+                  <c:v>6.039280873795317E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.2373487372281072E-2</c:v>
+                  <c:v>6.039280873795317E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.3609137631747582E-2</c:v>
+                  <c:v>-3.4741507318953639E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.3609137631747582E-2</c:v>
+                  <c:v>-3.4741507318953639E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.16211130541015681</c:v>
+                  <c:v>-0.16758290489215216</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.16211130541015681</c:v>
+                  <c:v>-0.16758290489215216</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-3.3646281336213321E-2</c:v>
+                  <c:v>-3.3385679140890294E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -27360,22 +27360,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:40" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AG1" s="476" t="s">
+      <c r="AG1" s="494" t="s">
         <v>113</v>
       </c>
-      <c r="AH1" s="476" t="s">
+      <c r="AH1" s="494" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" s="476" t="s">
+      <c r="AI1" s="494" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="476" t="s">
+      <c r="AJ1" s="494" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="470" t="s">
+      <c r="AK1" s="503" t="s">
         <v>57</v>
       </c>
-      <c r="AL1" s="470" t="s">
+      <c r="AL1" s="503" t="s">
         <v>52</v>
       </c>
     </row>
@@ -27452,23 +27452,23 @@
       <c r="Y2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AB2" s="473" t="s">
+      <c r="AB2" s="506" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="474"/>
-      <c r="AD2" s="477" t="s">
+      <c r="AC2" s="507"/>
+      <c r="AD2" s="501" t="s">
         <v>58</v>
       </c>
-      <c r="AE2" s="477"/>
+      <c r="AE2" s="501"/>
       <c r="AF2" s="95" t="s">
         <v>103</v>
       </c>
-      <c r="AG2" s="478"/>
-      <c r="AH2" s="476"/>
-      <c r="AI2" s="476"/>
-      <c r="AJ2" s="476"/>
-      <c r="AK2" s="470"/>
-      <c r="AL2" s="470"/>
+      <c r="AG2" s="509"/>
+      <c r="AH2" s="494"/>
+      <c r="AI2" s="494"/>
+      <c r="AJ2" s="494"/>
+      <c r="AK2" s="503"/>
+      <c r="AL2" s="503"/>
     </row>
     <row r="3" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B3" s="14">
@@ -29199,22 +29199,22 @@
       <c r="Y16" s="41">
         <v>1.1583636475738333</v>
       </c>
-      <c r="AG16" s="476" t="s">
+      <c r="AG16" s="494" t="s">
         <v>56</v>
       </c>
-      <c r="AH16" s="476" t="s">
+      <c r="AH16" s="494" t="s">
         <v>57</v>
       </c>
-      <c r="AI16" s="476" t="s">
+      <c r="AI16" s="494" t="s">
         <v>52</v>
       </c>
-      <c r="AJ16" s="476" t="s">
+      <c r="AJ16" s="494" t="s">
         <v>56</v>
       </c>
-      <c r="AK16" s="470" t="s">
+      <c r="AK16" s="503" t="s">
         <v>57</v>
       </c>
-      <c r="AL16" s="470" t="s">
+      <c r="AL16" s="503" t="s">
         <v>52</v>
       </c>
       <c r="AN16" s="379"/>
@@ -29293,23 +29293,23 @@
         <v>1.2284974412725813</v>
       </c>
       <c r="Z17" s="379"/>
-      <c r="AB17" s="473" t="s">
+      <c r="AB17" s="506" t="s">
         <v>40</v>
       </c>
-      <c r="AC17" s="475"/>
-      <c r="AD17" s="477" t="s">
+      <c r="AC17" s="508"/>
+      <c r="AD17" s="501" t="s">
         <v>58</v>
       </c>
-      <c r="AE17" s="477"/>
+      <c r="AE17" s="501"/>
       <c r="AF17" s="240" t="s">
         <v>103</v>
       </c>
-      <c r="AG17" s="476"/>
-      <c r="AH17" s="476"/>
-      <c r="AI17" s="476"/>
-      <c r="AJ17" s="476"/>
-      <c r="AK17" s="470"/>
-      <c r="AL17" s="470"/>
+      <c r="AG17" s="494"/>
+      <c r="AH17" s="494"/>
+      <c r="AI17" s="494"/>
+      <c r="AJ17" s="494"/>
+      <c r="AK17" s="503"/>
+      <c r="AL17" s="503"/>
       <c r="AN17" s="379"/>
     </row>
     <row r="18" spans="2:40" x14ac:dyDescent="0.25">
@@ -31018,14 +31018,14 @@
       <c r="Y32" s="41">
         <v>6.9971946482520506</v>
       </c>
-      <c r="AA32" s="471" t="s">
+      <c r="AA32" s="504" t="s">
         <v>25</v>
       </c>
-      <c r="AB32" s="471"/>
-      <c r="AC32" s="472" t="s">
+      <c r="AB32" s="504"/>
+      <c r="AC32" s="505" t="s">
         <v>40</v>
       </c>
-      <c r="AD32" s="472"/>
+      <c r="AD32" s="505"/>
       <c r="AI32" s="217" t="s">
         <v>76</v>
       </c>
@@ -32558,45 +32558,45 @@
       </c>
     </row>
     <row r="51" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="AA51" s="477" t="s">
+      <c r="AA51" s="501" t="s">
         <v>102</v>
       </c>
-      <c r="AB51" s="477"/>
-      <c r="AC51" s="477"/>
-      <c r="AD51" s="477"/>
-      <c r="AE51" s="477"/>
-      <c r="AF51" s="477"/>
-      <c r="AG51" s="477"/>
-      <c r="AH51" s="477"/>
-      <c r="AI51" s="477"/>
-      <c r="AJ51" s="477"/>
-      <c r="AK51" s="477"/>
-      <c r="AL51" s="477"/>
-      <c r="AM51" s="477"/>
-      <c r="AN51" s="477"/>
+      <c r="AB51" s="501"/>
+      <c r="AC51" s="501"/>
+      <c r="AD51" s="501"/>
+      <c r="AE51" s="501"/>
+      <c r="AF51" s="501"/>
+      <c r="AG51" s="501"/>
+      <c r="AH51" s="501"/>
+      <c r="AI51" s="501"/>
+      <c r="AJ51" s="501"/>
+      <c r="AK51" s="501"/>
+      <c r="AL51" s="501"/>
+      <c r="AM51" s="501"/>
+      <c r="AN51" s="501"/>
     </row>
     <row r="52" spans="2:40" x14ac:dyDescent="0.25">
       <c r="AA52" s="56"/>
-      <c r="AB52" s="488" t="s">
+      <c r="AB52" s="502" t="s">
         <v>72</v>
       </c>
-      <c r="AC52" s="488"/>
-      <c r="AD52" s="488"/>
-      <c r="AE52" s="488" t="s">
+      <c r="AC52" s="502"/>
+      <c r="AD52" s="502"/>
+      <c r="AE52" s="502" t="s">
         <v>73</v>
       </c>
-      <c r="AF52" s="488"/>
-      <c r="AG52" s="488"/>
-      <c r="AH52" s="488" t="s">
+      <c r="AF52" s="502"/>
+      <c r="AG52" s="502"/>
+      <c r="AH52" s="502" t="s">
         <v>74</v>
       </c>
-      <c r="AI52" s="488"/>
-      <c r="AJ52" s="488"/>
-      <c r="AK52" s="488" t="s">
+      <c r="AI52" s="502"/>
+      <c r="AJ52" s="502"/>
+      <c r="AK52" s="502" t="s">
         <v>75</v>
       </c>
-      <c r="AL52" s="488"/>
-      <c r="AM52" s="488"/>
+      <c r="AL52" s="502"/>
+      <c r="AM52" s="502"/>
       <c r="AN52" s="56"/>
     </row>
     <row r="53" spans="2:40" x14ac:dyDescent="0.25">
@@ -32691,34 +32691,34 @@
       </c>
     </row>
     <row r="55" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B55" s="485" t="s">
+      <c r="B55" s="498" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="486"/>
-      <c r="D55" s="486"/>
-      <c r="E55" s="486"/>
-      <c r="F55" s="487"/>
-      <c r="G55" s="485" t="s">
+      <c r="C55" s="499"/>
+      <c r="D55" s="499"/>
+      <c r="E55" s="499"/>
+      <c r="F55" s="500"/>
+      <c r="G55" s="498" t="s">
         <v>2</v>
       </c>
-      <c r="H55" s="486"/>
-      <c r="I55" s="486"/>
-      <c r="J55" s="486"/>
-      <c r="K55" s="487"/>
-      <c r="L55" s="485" t="s">
+      <c r="H55" s="499"/>
+      <c r="I55" s="499"/>
+      <c r="J55" s="499"/>
+      <c r="K55" s="500"/>
+      <c r="L55" s="498" t="s">
         <v>3</v>
       </c>
-      <c r="M55" s="486"/>
-      <c r="N55" s="486"/>
-      <c r="O55" s="486"/>
-      <c r="P55" s="487"/>
-      <c r="Q55" s="485" t="s">
+      <c r="M55" s="499"/>
+      <c r="N55" s="499"/>
+      <c r="O55" s="499"/>
+      <c r="P55" s="500"/>
+      <c r="Q55" s="498" t="s">
         <v>4</v>
       </c>
-      <c r="R55" s="486"/>
-      <c r="S55" s="486"/>
-      <c r="T55" s="486"/>
-      <c r="U55" s="487"/>
+      <c r="R55" s="499"/>
+      <c r="S55" s="499"/>
+      <c r="T55" s="499"/>
+      <c r="U55" s="500"/>
       <c r="AA55" s="206" t="s">
         <v>80</v>
       </c>
@@ -33929,20 +33929,20 @@
     </row>
     <row r="69" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B70" s="479" t="s">
+      <c r="B70" s="470" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="480"/>
-      <c r="D70" s="480"/>
-      <c r="E70" s="480"/>
-      <c r="F70" s="481"/>
-      <c r="G70" s="479" t="s">
+      <c r="C70" s="471"/>
+      <c r="D70" s="471"/>
+      <c r="E70" s="471"/>
+      <c r="F70" s="472"/>
+      <c r="G70" s="470" t="s">
         <v>6</v>
       </c>
-      <c r="H70" s="480"/>
-      <c r="I70" s="480"/>
-      <c r="J70" s="480"/>
-      <c r="K70" s="481"/>
+      <c r="H70" s="471"/>
+      <c r="I70" s="471"/>
+      <c r="J70" s="471"/>
+      <c r="K70" s="472"/>
     </row>
     <row r="71" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="146" t="s">
@@ -34350,20 +34350,20 @@
     </row>
     <row r="84" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B85" s="482" t="s">
+      <c r="B85" s="495" t="s">
         <v>7</v>
       </c>
-      <c r="C85" s="483"/>
-      <c r="D85" s="483"/>
-      <c r="E85" s="483"/>
-      <c r="F85" s="484"/>
-      <c r="G85" s="482" t="s">
+      <c r="C85" s="496"/>
+      <c r="D85" s="496"/>
+      <c r="E85" s="496"/>
+      <c r="F85" s="497"/>
+      <c r="G85" s="495" t="s">
         <v>8</v>
       </c>
-      <c r="H85" s="483"/>
-      <c r="I85" s="483"/>
-      <c r="J85" s="483"/>
-      <c r="K85" s="484"/>
+      <c r="H85" s="496"/>
+      <c r="I85" s="496"/>
+      <c r="J85" s="496"/>
+      <c r="K85" s="497"/>
     </row>
     <row r="86" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="161" t="s">
@@ -34773,34 +34773,34 @@
     </row>
     <row r="99" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="100" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B100" s="489" t="s">
+      <c r="B100" s="482" t="s">
         <v>9</v>
       </c>
-      <c r="C100" s="490"/>
-      <c r="D100" s="490"/>
-      <c r="E100" s="490"/>
-      <c r="F100" s="491"/>
-      <c r="G100" s="489" t="s">
+      <c r="C100" s="483"/>
+      <c r="D100" s="483"/>
+      <c r="E100" s="483"/>
+      <c r="F100" s="484"/>
+      <c r="G100" s="482" t="s">
         <v>10</v>
       </c>
-      <c r="H100" s="490"/>
-      <c r="I100" s="490"/>
-      <c r="J100" s="490"/>
-      <c r="K100" s="491"/>
-      <c r="L100" s="492" t="s">
+      <c r="H100" s="483"/>
+      <c r="I100" s="483"/>
+      <c r="J100" s="483"/>
+      <c r="K100" s="484"/>
+      <c r="L100" s="485" t="s">
         <v>11</v>
       </c>
-      <c r="M100" s="493"/>
-      <c r="N100" s="493"/>
-      <c r="O100" s="493"/>
-      <c r="P100" s="494"/>
-      <c r="Q100" s="489" t="s">
+      <c r="M100" s="486"/>
+      <c r="N100" s="486"/>
+      <c r="O100" s="486"/>
+      <c r="P100" s="487"/>
+      <c r="Q100" s="482" t="s">
         <v>12</v>
       </c>
-      <c r="R100" s="490"/>
-      <c r="S100" s="490"/>
-      <c r="T100" s="490"/>
-      <c r="U100" s="491"/>
+      <c r="R100" s="483"/>
+      <c r="S100" s="483"/>
+      <c r="T100" s="483"/>
+      <c r="U100" s="484"/>
     </row>
     <row r="101" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="171" t="s">
@@ -35588,34 +35588,34 @@
     </row>
     <row r="114" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="115" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B115" s="495" t="s">
+      <c r="B115" s="488" t="s">
         <v>13</v>
       </c>
-      <c r="C115" s="496"/>
-      <c r="D115" s="496"/>
-      <c r="E115" s="496"/>
-      <c r="F115" s="497"/>
-      <c r="G115" s="495" t="s">
+      <c r="C115" s="489"/>
+      <c r="D115" s="489"/>
+      <c r="E115" s="489"/>
+      <c r="F115" s="490"/>
+      <c r="G115" s="488" t="s">
         <v>14</v>
       </c>
-      <c r="H115" s="496"/>
-      <c r="I115" s="496"/>
-      <c r="J115" s="496"/>
-      <c r="K115" s="497"/>
-      <c r="L115" s="498" t="s">
+      <c r="H115" s="489"/>
+      <c r="I115" s="489"/>
+      <c r="J115" s="489"/>
+      <c r="K115" s="490"/>
+      <c r="L115" s="491" t="s">
         <v>15</v>
       </c>
-      <c r="M115" s="499"/>
-      <c r="N115" s="499"/>
-      <c r="O115" s="499"/>
-      <c r="P115" s="500"/>
-      <c r="Q115" s="495" t="s">
+      <c r="M115" s="492"/>
+      <c r="N115" s="492"/>
+      <c r="O115" s="492"/>
+      <c r="P115" s="493"/>
+      <c r="Q115" s="488" t="s">
         <v>16</v>
       </c>
-      <c r="R115" s="496"/>
-      <c r="S115" s="496"/>
-      <c r="T115" s="496"/>
-      <c r="U115" s="497"/>
+      <c r="R115" s="489"/>
+      <c r="S115" s="489"/>
+      <c r="T115" s="489"/>
+      <c r="U115" s="490"/>
     </row>
     <row r="116" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="181" t="s">
@@ -36403,34 +36403,34 @@
     </row>
     <row r="129" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="130" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B130" s="479" t="s">
+      <c r="B130" s="470" t="s">
         <v>17</v>
       </c>
-      <c r="C130" s="480"/>
-      <c r="D130" s="480"/>
-      <c r="E130" s="480"/>
-      <c r="F130" s="481"/>
-      <c r="G130" s="479" t="s">
+      <c r="C130" s="471"/>
+      <c r="D130" s="471"/>
+      <c r="E130" s="471"/>
+      <c r="F130" s="472"/>
+      <c r="G130" s="470" t="s">
         <v>18</v>
       </c>
-      <c r="H130" s="480"/>
-      <c r="I130" s="480"/>
-      <c r="J130" s="480"/>
-      <c r="K130" s="481"/>
-      <c r="L130" s="501" t="s">
+      <c r="H130" s="471"/>
+      <c r="I130" s="471"/>
+      <c r="J130" s="471"/>
+      <c r="K130" s="472"/>
+      <c r="L130" s="473" t="s">
         <v>19</v>
       </c>
-      <c r="M130" s="502"/>
-      <c r="N130" s="502"/>
-      <c r="O130" s="502"/>
-      <c r="P130" s="503"/>
-      <c r="Q130" s="479" t="s">
+      <c r="M130" s="474"/>
+      <c r="N130" s="474"/>
+      <c r="O130" s="474"/>
+      <c r="P130" s="475"/>
+      <c r="Q130" s="470" t="s">
         <v>20</v>
       </c>
-      <c r="R130" s="480"/>
-      <c r="S130" s="480"/>
-      <c r="T130" s="480"/>
-      <c r="U130" s="481"/>
+      <c r="R130" s="471"/>
+      <c r="S130" s="471"/>
+      <c r="T130" s="471"/>
+      <c r="U130" s="472"/>
     </row>
     <row r="131" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" s="146" t="s">
@@ -37218,27 +37218,27 @@
     </row>
     <row r="144" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="145" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B145" s="504" t="s">
+      <c r="B145" s="476" t="s">
         <v>21</v>
       </c>
-      <c r="C145" s="505"/>
-      <c r="D145" s="505"/>
-      <c r="E145" s="505"/>
-      <c r="F145" s="506"/>
-      <c r="G145" s="504" t="s">
+      <c r="C145" s="477"/>
+      <c r="D145" s="477"/>
+      <c r="E145" s="477"/>
+      <c r="F145" s="478"/>
+      <c r="G145" s="476" t="s">
         <v>22</v>
       </c>
-      <c r="H145" s="505"/>
-      <c r="I145" s="505"/>
-      <c r="J145" s="505"/>
-      <c r="K145" s="506"/>
-      <c r="L145" s="507" t="s">
+      <c r="H145" s="477"/>
+      <c r="I145" s="477"/>
+      <c r="J145" s="477"/>
+      <c r="K145" s="478"/>
+      <c r="L145" s="479" t="s">
         <v>23</v>
       </c>
-      <c r="M145" s="508"/>
-      <c r="N145" s="508"/>
-      <c r="O145" s="508"/>
-      <c r="P145" s="509"/>
+      <c r="M145" s="480"/>
+      <c r="N145" s="480"/>
+      <c r="O145" s="480"/>
+      <c r="P145" s="481"/>
     </row>
     <row r="146" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B146" s="191" t="s">
@@ -37837,36 +37837,6 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="G130:K130"/>
-    <mergeCell ref="L130:P130"/>
-    <mergeCell ref="Q130:U130"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="G145:K145"/>
-    <mergeCell ref="L145:P145"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="G100:K100"/>
-    <mergeCell ref="L100:P100"/>
-    <mergeCell ref="Q100:U100"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="G115:K115"/>
-    <mergeCell ref="L115:P115"/>
-    <mergeCell ref="Q115:U115"/>
-    <mergeCell ref="AH16:AH17"/>
-    <mergeCell ref="AI16:AI17"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="G70:K70"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="G85:K85"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="G55:K55"/>
-    <mergeCell ref="L55:P55"/>
-    <mergeCell ref="Q55:U55"/>
-    <mergeCell ref="AA51:AN51"/>
-    <mergeCell ref="AB52:AD52"/>
-    <mergeCell ref="AE52:AG52"/>
-    <mergeCell ref="AH52:AJ52"/>
-    <mergeCell ref="AK52:AM52"/>
     <mergeCell ref="AL1:AL2"/>
     <mergeCell ref="AL16:AL17"/>
     <mergeCell ref="AK16:AK17"/>
@@ -37883,6 +37853,36 @@
     <mergeCell ref="AH1:AH2"/>
     <mergeCell ref="AI1:AI2"/>
     <mergeCell ref="AG16:AG17"/>
+    <mergeCell ref="AH16:AH17"/>
+    <mergeCell ref="AI16:AI17"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="G70:K70"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="G85:K85"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="G55:K55"/>
+    <mergeCell ref="L55:P55"/>
+    <mergeCell ref="Q55:U55"/>
+    <mergeCell ref="AA51:AN51"/>
+    <mergeCell ref="AB52:AD52"/>
+    <mergeCell ref="AE52:AG52"/>
+    <mergeCell ref="AH52:AJ52"/>
+    <mergeCell ref="AK52:AM52"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="G100:K100"/>
+    <mergeCell ref="L100:P100"/>
+    <mergeCell ref="Q100:U100"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="G115:K115"/>
+    <mergeCell ref="L115:P115"/>
+    <mergeCell ref="Q115:U115"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="G130:K130"/>
+    <mergeCell ref="L130:P130"/>
+    <mergeCell ref="Q130:U130"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="G145:K145"/>
+    <mergeCell ref="L145:P145"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -37918,22 +37918,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="AG1" s="476" t="s">
+      <c r="AG1" s="494" t="s">
         <v>113</v>
       </c>
-      <c r="AH1" s="476" t="s">
+      <c r="AH1" s="494" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" s="476" t="s">
+      <c r="AI1" s="494" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="476" t="s">
+      <c r="AJ1" s="494" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="476" t="s">
+      <c r="AK1" s="494" t="s">
         <v>57</v>
       </c>
-      <c r="AL1" s="476" t="s">
+      <c r="AL1" s="494" t="s">
         <v>52</v>
       </c>
     </row>
@@ -38010,23 +38010,23 @@
       <c r="Y2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AB2" s="473" t="s">
+      <c r="AB2" s="506" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="474"/>
-      <c r="AD2" s="477" t="s">
+      <c r="AC2" s="507"/>
+      <c r="AD2" s="501" t="s">
         <v>58</v>
       </c>
-      <c r="AE2" s="477"/>
+      <c r="AE2" s="501"/>
       <c r="AF2" s="95" t="s">
         <v>103</v>
       </c>
-      <c r="AG2" s="476"/>
-      <c r="AH2" s="476"/>
-      <c r="AI2" s="476"/>
-      <c r="AJ2" s="476"/>
-      <c r="AK2" s="476"/>
-      <c r="AL2" s="476"/>
+      <c r="AG2" s="494"/>
+      <c r="AH2" s="494"/>
+      <c r="AI2" s="494"/>
+      <c r="AJ2" s="494"/>
+      <c r="AK2" s="494"/>
+      <c r="AL2" s="494"/>
     </row>
     <row r="3" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B3" s="14">
@@ -39567,22 +39567,22 @@
       <c r="Y15" s="315">
         <v>1.0235026535253984</v>
       </c>
-      <c r="AG15" s="476" t="s">
+      <c r="AG15" s="494" t="s">
         <v>56</v>
       </c>
-      <c r="AH15" s="476" t="s">
+      <c r="AH15" s="494" t="s">
         <v>57</v>
       </c>
-      <c r="AI15" s="476" t="s">
+      <c r="AI15" s="494" t="s">
         <v>52</v>
       </c>
-      <c r="AJ15" s="476" t="s">
+      <c r="AJ15" s="494" t="s">
         <v>56</v>
       </c>
-      <c r="AK15" s="476" t="s">
+      <c r="AK15" s="494" t="s">
         <v>57</v>
       </c>
-      <c r="AL15" s="476" t="s">
+      <c r="AL15" s="494" t="s">
         <v>52</v>
       </c>
       <c r="AM15" s="381"/>
@@ -39659,23 +39659,23 @@
       <c r="Y16" s="315">
         <v>1.0708870356330553</v>
       </c>
-      <c r="AB16" s="473" t="s">
+      <c r="AB16" s="506" t="s">
         <v>40</v>
       </c>
-      <c r="AC16" s="475"/>
-      <c r="AD16" s="477" t="s">
+      <c r="AC16" s="508"/>
+      <c r="AD16" s="501" t="s">
         <v>58</v>
       </c>
-      <c r="AE16" s="477"/>
+      <c r="AE16" s="501"/>
       <c r="AF16" s="95" t="s">
         <v>103</v>
       </c>
-      <c r="AG16" s="476"/>
-      <c r="AH16" s="476"/>
-      <c r="AI16" s="476"/>
-      <c r="AJ16" s="476"/>
-      <c r="AK16" s="476"/>
-      <c r="AL16" s="476"/>
+      <c r="AG16" s="494"/>
+      <c r="AH16" s="494"/>
+      <c r="AI16" s="494"/>
+      <c r="AJ16" s="494"/>
+      <c r="AK16" s="494"/>
+      <c r="AL16" s="494"/>
       <c r="AM16" s="381"/>
       <c r="AN16" s="381"/>
     </row>
@@ -41356,14 +41356,14 @@
       <c r="Y31" s="315">
         <v>6.6148597422289619</v>
       </c>
-      <c r="AA31" s="471" t="s">
+      <c r="AA31" s="504" t="s">
         <v>25</v>
       </c>
-      <c r="AB31" s="471"/>
-      <c r="AC31" s="472" t="s">
+      <c r="AB31" s="504"/>
+      <c r="AC31" s="505" t="s">
         <v>40</v>
       </c>
-      <c r="AD31" s="472"/>
+      <c r="AD31" s="505"/>
       <c r="AJ31" s="217" t="s">
         <v>76</v>
       </c>
@@ -43744,20 +43744,20 @@
       </c>
     </row>
     <row r="70" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="501" t="s">
+      <c r="B70" s="473" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="502"/>
-      <c r="D70" s="502"/>
-      <c r="E70" s="502"/>
-      <c r="F70" s="503"/>
-      <c r="G70" s="501" t="s">
+      <c r="C70" s="474"/>
+      <c r="D70" s="474"/>
+      <c r="E70" s="474"/>
+      <c r="F70" s="475"/>
+      <c r="G70" s="473" t="s">
         <v>6</v>
       </c>
-      <c r="H70" s="502"/>
-      <c r="I70" s="502"/>
-      <c r="J70" s="502"/>
-      <c r="K70" s="503"/>
+      <c r="H70" s="474"/>
+      <c r="I70" s="474"/>
+      <c r="J70" s="474"/>
+      <c r="K70" s="475"/>
       <c r="R70" s="388" t="s">
         <v>111</v>
       </c>
@@ -45052,34 +45052,34 @@
     </row>
     <row r="99" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="100" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B100" s="492" t="s">
+      <c r="B100" s="485" t="s">
         <v>9</v>
       </c>
-      <c r="C100" s="493"/>
-      <c r="D100" s="493"/>
-      <c r="E100" s="493"/>
-      <c r="F100" s="494"/>
-      <c r="G100" s="492" t="s">
+      <c r="C100" s="486"/>
+      <c r="D100" s="486"/>
+      <c r="E100" s="486"/>
+      <c r="F100" s="487"/>
+      <c r="G100" s="485" t="s">
         <v>10</v>
       </c>
-      <c r="H100" s="493"/>
-      <c r="I100" s="493"/>
-      <c r="J100" s="493"/>
-      <c r="K100" s="494"/>
-      <c r="L100" s="492" t="s">
+      <c r="H100" s="486"/>
+      <c r="I100" s="486"/>
+      <c r="J100" s="486"/>
+      <c r="K100" s="487"/>
+      <c r="L100" s="485" t="s">
         <v>11</v>
       </c>
-      <c r="M100" s="493"/>
-      <c r="N100" s="493"/>
-      <c r="O100" s="493"/>
-      <c r="P100" s="494"/>
-      <c r="Q100" s="492" t="s">
+      <c r="M100" s="486"/>
+      <c r="N100" s="486"/>
+      <c r="O100" s="486"/>
+      <c r="P100" s="487"/>
+      <c r="Q100" s="485" t="s">
         <v>12</v>
       </c>
-      <c r="R100" s="493"/>
-      <c r="S100" s="493"/>
-      <c r="T100" s="493"/>
-      <c r="U100" s="494"/>
+      <c r="R100" s="486"/>
+      <c r="S100" s="486"/>
+      <c r="T100" s="486"/>
+      <c r="U100" s="487"/>
     </row>
     <row r="101" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="171" t="s">
@@ -45867,34 +45867,34 @@
     </row>
     <row r="114" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="115" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B115" s="495" t="s">
+      <c r="B115" s="488" t="s">
         <v>13</v>
       </c>
-      <c r="C115" s="496"/>
-      <c r="D115" s="496"/>
-      <c r="E115" s="496"/>
-      <c r="F115" s="497"/>
-      <c r="G115" s="498" t="s">
+      <c r="C115" s="489"/>
+      <c r="D115" s="489"/>
+      <c r="E115" s="489"/>
+      <c r="F115" s="490"/>
+      <c r="G115" s="491" t="s">
         <v>14</v>
       </c>
-      <c r="H115" s="499"/>
-      <c r="I115" s="499"/>
-      <c r="J115" s="499"/>
-      <c r="K115" s="500"/>
-      <c r="L115" s="498" t="s">
+      <c r="H115" s="492"/>
+      <c r="I115" s="492"/>
+      <c r="J115" s="492"/>
+      <c r="K115" s="493"/>
+      <c r="L115" s="491" t="s">
         <v>15</v>
       </c>
-      <c r="M115" s="499"/>
-      <c r="N115" s="499"/>
-      <c r="O115" s="499"/>
-      <c r="P115" s="500"/>
-      <c r="Q115" s="498" t="s">
+      <c r="M115" s="492"/>
+      <c r="N115" s="492"/>
+      <c r="O115" s="492"/>
+      <c r="P115" s="493"/>
+      <c r="Q115" s="491" t="s">
         <v>16</v>
       </c>
-      <c r="R115" s="499"/>
-      <c r="S115" s="499"/>
-      <c r="T115" s="499"/>
-      <c r="U115" s="500"/>
+      <c r="R115" s="492"/>
+      <c r="S115" s="492"/>
+      <c r="T115" s="492"/>
+      <c r="U115" s="493"/>
     </row>
     <row r="116" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="181" t="s">
@@ -46566,34 +46566,34 @@
     </row>
     <row r="129" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="130" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B130" s="501" t="s">
+      <c r="B130" s="473" t="s">
         <v>17</v>
       </c>
-      <c r="C130" s="502"/>
-      <c r="D130" s="502"/>
-      <c r="E130" s="502"/>
-      <c r="F130" s="503"/>
-      <c r="G130" s="501" t="s">
+      <c r="C130" s="474"/>
+      <c r="D130" s="474"/>
+      <c r="E130" s="474"/>
+      <c r="F130" s="475"/>
+      <c r="G130" s="473" t="s">
         <v>18</v>
       </c>
-      <c r="H130" s="502"/>
-      <c r="I130" s="502"/>
-      <c r="J130" s="502"/>
-      <c r="K130" s="503"/>
-      <c r="L130" s="501" t="s">
+      <c r="H130" s="474"/>
+      <c r="I130" s="474"/>
+      <c r="J130" s="474"/>
+      <c r="K130" s="475"/>
+      <c r="L130" s="473" t="s">
         <v>19</v>
       </c>
-      <c r="M130" s="502"/>
-      <c r="N130" s="502"/>
-      <c r="O130" s="502"/>
-      <c r="P130" s="503"/>
-      <c r="Q130" s="501" t="s">
+      <c r="M130" s="474"/>
+      <c r="N130" s="474"/>
+      <c r="O130" s="474"/>
+      <c r="P130" s="475"/>
+      <c r="Q130" s="473" t="s">
         <v>20</v>
       </c>
-      <c r="R130" s="502"/>
-      <c r="S130" s="502"/>
-      <c r="T130" s="502"/>
-      <c r="U130" s="503"/>
+      <c r="R130" s="474"/>
+      <c r="S130" s="474"/>
+      <c r="T130" s="474"/>
+      <c r="U130" s="475"/>
     </row>
     <row r="131" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" s="146" t="s">
@@ -47381,27 +47381,27 @@
     </row>
     <row r="144" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="145" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B145" s="507" t="s">
+      <c r="B145" s="479" t="s">
         <v>21</v>
       </c>
-      <c r="C145" s="508"/>
-      <c r="D145" s="508"/>
-      <c r="E145" s="508"/>
-      <c r="F145" s="509"/>
-      <c r="G145" s="507" t="s">
+      <c r="C145" s="480"/>
+      <c r="D145" s="480"/>
+      <c r="E145" s="480"/>
+      <c r="F145" s="481"/>
+      <c r="G145" s="479" t="s">
         <v>22</v>
       </c>
-      <c r="H145" s="508"/>
-      <c r="I145" s="508"/>
-      <c r="J145" s="508"/>
-      <c r="K145" s="509"/>
-      <c r="L145" s="507" t="s">
+      <c r="H145" s="480"/>
+      <c r="I145" s="480"/>
+      <c r="J145" s="480"/>
+      <c r="K145" s="481"/>
+      <c r="L145" s="479" t="s">
         <v>23</v>
       </c>
-      <c r="M145" s="508"/>
-      <c r="N145" s="508"/>
-      <c r="O145" s="508"/>
-      <c r="P145" s="509"/>
+      <c r="M145" s="480"/>
+      <c r="N145" s="480"/>
+      <c r="O145" s="480"/>
+      <c r="P145" s="481"/>
     </row>
     <row r="146" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B146" s="191" t="s">
@@ -48000,17 +48000,24 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="G145:K145"/>
-    <mergeCell ref="L145:P145"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="G115:K115"/>
-    <mergeCell ref="L115:P115"/>
-    <mergeCell ref="Q115:U115"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="G130:K130"/>
-    <mergeCell ref="L130:P130"/>
-    <mergeCell ref="Q130:U130"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="AK15:AK16"/>
+    <mergeCell ref="AL15:AL16"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AD16:AE16"/>
+    <mergeCell ref="AA31:AB31"/>
+    <mergeCell ref="AC31:AD31"/>
+    <mergeCell ref="AJ15:AJ16"/>
+    <mergeCell ref="AG15:AG16"/>
+    <mergeCell ref="AH15:AH16"/>
+    <mergeCell ref="AI15:AI16"/>
     <mergeCell ref="Q100:U100"/>
     <mergeCell ref="B55:F55"/>
     <mergeCell ref="G55:K55"/>
@@ -48023,24 +48030,17 @@
     <mergeCell ref="B100:F100"/>
     <mergeCell ref="G100:K100"/>
     <mergeCell ref="L100:P100"/>
-    <mergeCell ref="AK15:AK16"/>
-    <mergeCell ref="AL15:AL16"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AD16:AE16"/>
-    <mergeCell ref="AA31:AB31"/>
-    <mergeCell ref="AC31:AD31"/>
-    <mergeCell ref="AJ15:AJ16"/>
-    <mergeCell ref="AG15:AG16"/>
-    <mergeCell ref="AH15:AH16"/>
-    <mergeCell ref="AI15:AI16"/>
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="AH1:AH2"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="Q115:U115"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="G130:K130"/>
+    <mergeCell ref="L130:P130"/>
+    <mergeCell ref="Q130:U130"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="G145:K145"/>
+    <mergeCell ref="L145:P145"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="G115:K115"/>
+    <mergeCell ref="L115:P115"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -48052,8 +48052,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" topLeftCell="I12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P44" sqref="P44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48074,22 +48074,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="477" t="s">
+      <c r="A1" s="501" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="520"/>
-      <c r="C1" s="520"/>
-      <c r="D1" s="520"/>
-      <c r="E1" s="520"/>
-      <c r="F1" s="520"/>
-      <c r="G1" s="520"/>
-      <c r="H1" s="520"/>
-      <c r="I1" s="520"/>
-      <c r="J1" s="520"/>
-      <c r="K1" s="520"/>
-      <c r="L1" s="520"/>
-      <c r="M1" s="520"/>
-      <c r="N1" s="477"/>
+      <c r="B1" s="516"/>
+      <c r="C1" s="516"/>
+      <c r="D1" s="516"/>
+      <c r="E1" s="516"/>
+      <c r="F1" s="516"/>
+      <c r="G1" s="516"/>
+      <c r="H1" s="516"/>
+      <c r="I1" s="516"/>
+      <c r="J1" s="516"/>
+      <c r="K1" s="516"/>
+      <c r="L1" s="516"/>
+      <c r="M1" s="516"/>
+      <c r="N1" s="501"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="216"/>
@@ -48114,11 +48114,11 @@
       <c r="L2" s="518"/>
       <c r="M2" s="519"/>
       <c r="N2" s="232"/>
-      <c r="O2" s="516" t="s">
+      <c r="O2" s="520" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="516"/>
-      <c r="Q2" s="516"/>
+      <c r="P2" s="520"/>
+      <c r="Q2" s="520"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="217" t="s">
@@ -48232,10 +48232,10 @@
         <v>0.2230334321880649</v>
       </c>
       <c r="P4" s="86">
-        <v>0.18882498202240408</v>
+        <v>0.20455321949518118</v>
       </c>
       <c r="Q4" s="86">
-        <v>0.22907037862867247</v>
+        <v>0.20454360227175514</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -48297,10 +48297,10 @@
         <v>0.2230334321880649</v>
       </c>
       <c r="P5" s="86">
-        <v>0.18882498202240408</v>
+        <v>0.20455321949518118</v>
       </c>
       <c r="Q5" s="86">
-        <v>0.22907037862867247</v>
+        <v>0.20454360227175514</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -48362,10 +48362,10 @@
         <v>-0.31265838987341704</v>
       </c>
       <c r="P6" s="208">
-        <v>-0.32061441221680753</v>
+        <v>-0.31662176778338602</v>
       </c>
       <c r="Q6" s="208">
-        <v>-0.31502368370436307</v>
+        <v>-0.31661374974045781</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -48427,10 +48427,10 @@
         <v>-8.6110173743218735E-2</v>
       </c>
       <c r="P7" s="210">
-        <v>-0.11450901614105548</v>
+        <v>-0.11018080455254639</v>
       </c>
       <c r="Q7" s="210">
-        <v>-7.346940523597506E-2</v>
+        <v>-0.11017208412824342</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -48492,10 +48492,10 @@
         <v>5.3443295479204331E-2</v>
       </c>
       <c r="P8" s="87">
-        <v>6.2373487372281072E-2</v>
+        <v>6.039280873795317E-2</v>
       </c>
       <c r="Q8" s="87">
-        <v>4.909818870881559E-2</v>
+        <v>6.0405779541984679E-2</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -48557,10 +48557,10 @@
         <v>5.3443295479204331E-2</v>
       </c>
       <c r="P9" s="87">
-        <v>6.2373487372281072E-2</v>
+        <v>6.039280873795317E-2</v>
       </c>
       <c r="Q9" s="87">
-        <v>4.909818870881559E-2</v>
+        <v>6.0405779541984679E-2</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -48622,10 +48622,10 @@
         <v>-3.8375210126582203E-2</v>
       </c>
       <c r="P10" s="213">
-        <v>-3.3609137631747582E-2</v>
+        <v>-3.4741507318953639E-2</v>
       </c>
       <c r="Q10" s="213">
-        <v>-3.9825588886910034E-2</v>
+        <v>-3.4732918409770948E-2</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -48687,10 +48687,10 @@
         <v>-3.8375210126582203E-2</v>
       </c>
       <c r="P11" s="213">
-        <v>-3.3609137631747582E-2</v>
+        <v>-3.4741507318953639E-2</v>
       </c>
       <c r="Q11" s="213">
-        <v>-3.9825588886910034E-2</v>
+        <v>-3.4732918409770948E-2</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -48752,10 +48752,10 @@
         <v>-0.14280064578661794</v>
       </c>
       <c r="P12" s="208">
-        <v>-0.16211130541015681</v>
+        <v>-0.16758290489215216</v>
       </c>
       <c r="Q12" s="208">
-        <v>-0.10258748751558326</v>
+        <v>-0.16746416727938898</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -48817,10 +48817,10 @@
         <v>-0.14280064578661794</v>
       </c>
       <c r="P13" s="208">
-        <v>-0.16211130541015681</v>
+        <v>-0.16758290489215216</v>
       </c>
       <c r="Q13" s="208">
-        <v>-0.10258748751558326</v>
+        <v>-0.16746416727938898</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -48882,10 +48882,10 @@
         <v>-3.5635726524412284E-2</v>
       </c>
       <c r="P14" s="215">
-        <v>-3.3646281336213321E-2</v>
+        <v>-3.3385679140890294E-2</v>
       </c>
       <c r="Q14" s="215">
-        <v>-3.883410208370431E-2</v>
+        <v>-3.3378369109007613E-2</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -48894,22 +48894,22 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="477" t="s">
+      <c r="A16" s="501" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="520"/>
-      <c r="C16" s="520"/>
-      <c r="D16" s="520"/>
-      <c r="E16" s="520"/>
-      <c r="F16" s="520"/>
-      <c r="G16" s="520"/>
-      <c r="H16" s="520"/>
-      <c r="I16" s="520"/>
-      <c r="J16" s="520"/>
-      <c r="K16" s="520"/>
-      <c r="L16" s="520"/>
-      <c r="M16" s="520"/>
-      <c r="N16" s="477"/>
+      <c r="B16" s="516"/>
+      <c r="C16" s="516"/>
+      <c r="D16" s="516"/>
+      <c r="E16" s="516"/>
+      <c r="F16" s="516"/>
+      <c r="G16" s="516"/>
+      <c r="H16" s="516"/>
+      <c r="I16" s="516"/>
+      <c r="J16" s="516"/>
+      <c r="K16" s="516"/>
+      <c r="L16" s="516"/>
+      <c r="M16" s="516"/>
+      <c r="N16" s="501"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="216"/>
@@ -48934,11 +48934,11 @@
       <c r="L17" s="518"/>
       <c r="M17" s="519"/>
       <c r="N17" s="232"/>
-      <c r="O17" s="516" t="s">
+      <c r="O17" s="520" t="s">
         <v>27</v>
       </c>
-      <c r="P17" s="516"/>
-      <c r="Q17" s="516"/>
+      <c r="P17" s="520"/>
+      <c r="Q17" s="520"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="217" t="s">
@@ -49052,10 +49052,10 @@
         <v>-0.25426105257495052</v>
       </c>
       <c r="P19" s="86">
-        <v>-0.20417995461623964</v>
+        <v>-0.23784858917921259</v>
       </c>
       <c r="Q19" s="86">
-        <v>-0.21250269512953343</v>
+        <v>-0.25646381521666273</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -49117,10 +49117,10 @@
         <v>-0.25426105257495052</v>
       </c>
       <c r="P20" s="86">
-        <v>-0.20417995461623964</v>
+        <v>-0.23784858917921259</v>
       </c>
       <c r="Q20" s="86">
-        <v>-0.21250269512953343</v>
+        <v>-0.25646381521666273</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -49182,10 +49182,10 @@
         <v>-0.32588985777528645</v>
       </c>
       <c r="P21" s="466">
-        <v>-0.31261653570633985</v>
+        <v>-0.32194296104905268</v>
       </c>
       <c r="Q21" s="466">
-        <v>-0.31338709554404104</v>
+        <v>-0.32648441197031308</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -49247,10 +49247,10 @@
         <v>9.0511453785373924E-2</v>
       </c>
       <c r="P22" s="87">
-        <v>0.11724795870967698</v>
+        <v>9.8870595823215071E-2</v>
       </c>
       <c r="Q22" s="87">
-        <v>0.11558307282901517</v>
+        <v>8.8871890830739209E-2</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -49312,10 +49312,10 @@
         <v>9.0511453785373924E-2</v>
       </c>
       <c r="P23" s="87">
-        <v>0.11724795870967698</v>
+        <v>9.8870595823215071E-2</v>
       </c>
       <c r="Q23" s="87">
-        <v>0.11558307282901517</v>
+        <v>8.8871890830739209E-2</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -49377,10 +49377,10 @@
         <v>-5.7166053639674974E-2</v>
       </c>
       <c r="P24" s="213">
-        <v>-4.048383003337034E-2</v>
+        <v>-5.1068450937348228E-2</v>
       </c>
       <c r="Q24" s="213">
-        <v>-4.1403888746113962E-2</v>
+        <v>-5.8003155872635853E-2</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -49442,10 +49442,10 @@
         <v>-0.12387199390305322</v>
       </c>
       <c r="P25" s="208">
-        <v>-0.1076174245161288</v>
+        <v>-0.12059113340456466</v>
       </c>
       <c r="Q25" s="208">
-        <v>-0.10857605372020686</v>
+        <v>-0.12379754395977956</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -49507,10 +49507,10 @@
         <v>-0.12387199390305322</v>
       </c>
       <c r="P26" s="208">
-        <v>-0.1076174245161288</v>
+        <v>-0.12059113340456466</v>
       </c>
       <c r="Q26" s="208">
-        <v>-0.10857605372020686</v>
+        <v>-0.12379754395977956</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -49572,29 +49572,29 @@
         <v>-5.2281245372933521E-2</v>
       </c>
       <c r="P27" s="215">
-        <v>-4.730072532146827E-2</v>
+        <v>-5.0699230181641519E-2</v>
       </c>
       <c r="Q27" s="215">
-        <v>-4.7612346826943E-2</v>
+        <v>-5.2460135362221633E-2</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="477" t="s">
+      <c r="A29" s="501" t="s">
         <v>106</v>
       </c>
-      <c r="B29" s="520"/>
-      <c r="C29" s="520"/>
-      <c r="D29" s="520"/>
-      <c r="E29" s="520"/>
-      <c r="F29" s="520"/>
-      <c r="G29" s="520"/>
-      <c r="H29" s="520"/>
-      <c r="I29" s="520"/>
-      <c r="J29" s="520"/>
-      <c r="K29" s="520"/>
-      <c r="L29" s="520"/>
-      <c r="M29" s="520"/>
-      <c r="N29" s="477"/>
+      <c r="B29" s="516"/>
+      <c r="C29" s="516"/>
+      <c r="D29" s="516"/>
+      <c r="E29" s="516"/>
+      <c r="F29" s="516"/>
+      <c r="G29" s="516"/>
+      <c r="H29" s="516"/>
+      <c r="I29" s="516"/>
+      <c r="J29" s="516"/>
+      <c r="K29" s="516"/>
+      <c r="L29" s="516"/>
+      <c r="M29" s="516"/>
+      <c r="N29" s="501"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="216"/>
@@ -49619,11 +49619,11 @@
       <c r="L30" s="518"/>
       <c r="M30" s="519"/>
       <c r="N30" s="232"/>
-      <c r="O30" s="516" t="s">
+      <c r="O30" s="520" t="s">
         <v>27</v>
       </c>
-      <c r="P30" s="516"/>
-      <c r="Q30" s="516"/>
+      <c r="P30" s="520"/>
+      <c r="Q30" s="520"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="217" t="s">
@@ -49737,10 +49737,10 @@
         <v>-0.25426105257495052</v>
       </c>
       <c r="P32" s="86">
-        <v>-0.20417995461623964</v>
+        <v>-0.23784858917921259</v>
       </c>
       <c r="Q32" s="86">
-        <v>-0.21250269512953343</v>
+        <v>-0.25646381521666273</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -49802,10 +49802,10 @@
         <v>-0.32588985777528645</v>
       </c>
       <c r="P33" s="466">
-        <v>-0.31261653570633985</v>
+        <v>-0.32194296104905268</v>
       </c>
       <c r="Q33" s="466">
-        <v>-0.31338709554404104</v>
+        <v>-0.32648441197031308</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -49867,10 +49867,10 @@
         <v>9.0511453785373924E-2</v>
       </c>
       <c r="P34" s="87">
-        <v>0.11724795870967698</v>
+        <v>9.8870595823215071E-2</v>
       </c>
       <c r="Q34" s="87">
-        <v>0.11558307282901517</v>
+        <v>8.8871890830739209E-2</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -49932,10 +49932,10 @@
         <v>9.0511453785373924E-2</v>
       </c>
       <c r="P35" s="87">
-        <v>0.11724795870967698</v>
+        <v>9.8870595823215071E-2</v>
       </c>
       <c r="Q35" s="87">
-        <v>0.11558307282901517</v>
+        <v>8.8871890830739209E-2</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -49997,10 +49997,10 @@
         <v>-5.7166053639674974E-2</v>
       </c>
       <c r="P36" s="213">
-        <v>-4.048383003337034E-2</v>
+        <v>-5.1068450937348228E-2</v>
       </c>
       <c r="Q36" s="213">
-        <v>-4.1403888746113962E-2</v>
+        <v>-5.8003155872635853E-2</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -50062,10 +50062,10 @@
         <v>-0.12387199390305322</v>
       </c>
       <c r="P37" s="208">
-        <v>-0.1076174245161288</v>
+        <v>-0.12059113340456466</v>
       </c>
       <c r="Q37" s="208">
-        <v>-0.10857605372020686</v>
+        <v>-0.12379754395977956</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -50127,10 +50127,10 @@
         <v>-0.12387199390305322</v>
       </c>
       <c r="P38" s="208">
-        <v>-0.1076174245161288</v>
+        <v>-0.12059113340456466</v>
       </c>
       <c r="Q38" s="208">
-        <v>-0.10857605372020686</v>
+        <v>-0.12379754395977956</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -50192,19 +50192,14 @@
         <v>-5.2281245372933521E-2</v>
       </c>
       <c r="P39" s="215">
-        <v>-4.730072532146827E-2</v>
+        <v>-5.0699230181641519E-2</v>
       </c>
       <c r="Q39" s="215">
-        <v>-4.7612346826943E-2</v>
+        <v>-5.2460135362221633E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
     <mergeCell ref="O2:Q2"/>
     <mergeCell ref="O17:Q17"/>
     <mergeCell ref="O30:Q30"/>
@@ -50218,6 +50213,11 @@
     <mergeCell ref="E30:G30"/>
     <mergeCell ref="H30:J30"/>
     <mergeCell ref="K30:M30"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
i want to kill myself :)
</commit_message>
<xml_diff>
--- a/GSD/baskets_new_sizes/basketGSD_hypflux_CS1mm.xlsx
+++ b/GSD/baskets_new_sizes/basketGSD_hypflux_CS1mm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\baskets_new_sizes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C3B1C5-1617-4541-9B71-CE6F7B8FA031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE394BAF-8F41-484F-8A71-EAE195264457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{FF2C68C4-0230-4397-BD30-01ABAA0FCBBF}"/>
+    <workbookView minimized="1" xWindow="-25200" yWindow="450" windowWidth="25200" windowHeight="15150" activeTab="3" xr2:uid="{FF2C68C4-0230-4397-BD30-01ABAA0FCBBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Spring Weights" sheetId="1" r:id="rId1"/>
@@ -2815,33 +2815,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="31" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2851,25 +2824,31 @@
     <xf numFmtId="0" fontId="0" fillId="31" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="29" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2908,32 +2887,53 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2953,7 +2953,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2965,7 +2965,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -18877,8 +18877,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.22618477007469806"/>
-                  <c:y val="-0.46126078522228348"/>
+                  <c:x val="-0.33197033885871308"/>
+                  <c:y val="-0.34350074081702198"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -18928,9 +18928,6 @@
                 <c:pt idx="1">
                   <c:v>-0.10058679002726996</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.32001589401318498</c:v>
-                </c:pt>
                 <c:pt idx="3">
                   <c:v>0.11743877238132332</c:v>
                 </c:pt>
@@ -19047,8 +19044,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.31262354239282519"/>
-                  <c:y val="7.4311478693756997E-2"/>
+                  <c:x val="-0.34595785170296911"/>
+                  <c:y val="0.11530364241303283"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -19098,9 +19095,6 @@
                 <c:pt idx="1">
                   <c:v>-0.10058679002726996</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.32001589401318498</c:v>
-                </c:pt>
                 <c:pt idx="3">
                   <c:v>0.11743877238132332</c:v>
                 </c:pt>
@@ -19217,8 +19211,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="8.7139025849171936E-2"/>
-                  <c:y val="-0.35826724197487542"/>
+                  <c:x val="9.7316134201240315E-2"/>
+                  <c:y val="-0.14966270932704029"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -19268,9 +19262,6 @@
                 <c:pt idx="1">
                   <c:v>-0.10058679002726996</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.32001589401318498</c:v>
-                </c:pt>
                 <c:pt idx="3">
                   <c:v>0.11743877238132332</c:v>
                 </c:pt>
@@ -19387,8 +19378,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="9.897448852042319E-2"/>
-                  <c:y val="-0.26404120389226238"/>
+                  <c:x val="2.7489450933091984E-2"/>
+                  <c:y val="0.12934358578580119"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -19437,9 +19428,6 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-0.10058679002726996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.32001589401318498</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.11743877238132332</c:v>
@@ -37892,22 +37880,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:40" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AG1" s="477" t="s">
+      <c r="AG1" s="495" t="s">
         <v>113</v>
       </c>
-      <c r="AH1" s="477" t="s">
+      <c r="AH1" s="495" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" s="477" t="s">
+      <c r="AI1" s="495" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="477" t="s">
+      <c r="AJ1" s="495" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="471" t="s">
+      <c r="AK1" s="504" t="s">
         <v>57</v>
       </c>
-      <c r="AL1" s="471" t="s">
+      <c r="AL1" s="504" t="s">
         <v>52</v>
       </c>
     </row>
@@ -37984,23 +37972,23 @@
       <c r="Y2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AB2" s="474" t="s">
+      <c r="AB2" s="507" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="475"/>
-      <c r="AD2" s="478" t="s">
+      <c r="AC2" s="508"/>
+      <c r="AD2" s="502" t="s">
         <v>58</v>
       </c>
-      <c r="AE2" s="478"/>
+      <c r="AE2" s="502"/>
       <c r="AF2" s="95" t="s">
         <v>103</v>
       </c>
-      <c r="AG2" s="479"/>
-      <c r="AH2" s="477"/>
-      <c r="AI2" s="477"/>
-      <c r="AJ2" s="477"/>
-      <c r="AK2" s="471"/>
-      <c r="AL2" s="471"/>
+      <c r="AG2" s="510"/>
+      <c r="AH2" s="495"/>
+      <c r="AI2" s="495"/>
+      <c r="AJ2" s="495"/>
+      <c r="AK2" s="504"/>
+      <c r="AL2" s="504"/>
     </row>
     <row r="3" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B3" s="14">
@@ -39731,22 +39719,22 @@
       <c r="Y16" s="41">
         <v>1.1583636475738333</v>
       </c>
-      <c r="AG16" s="477" t="s">
+      <c r="AG16" s="495" t="s">
         <v>56</v>
       </c>
-      <c r="AH16" s="477" t="s">
+      <c r="AH16" s="495" t="s">
         <v>57</v>
       </c>
-      <c r="AI16" s="477" t="s">
+      <c r="AI16" s="495" t="s">
         <v>52</v>
       </c>
-      <c r="AJ16" s="477" t="s">
+      <c r="AJ16" s="495" t="s">
         <v>56</v>
       </c>
-      <c r="AK16" s="471" t="s">
+      <c r="AK16" s="504" t="s">
         <v>57</v>
       </c>
-      <c r="AL16" s="471" t="s">
+      <c r="AL16" s="504" t="s">
         <v>52</v>
       </c>
       <c r="AN16" s="379"/>
@@ -39825,23 +39813,23 @@
         <v>1.2284974412725813</v>
       </c>
       <c r="Z17" s="379"/>
-      <c r="AB17" s="474" t="s">
+      <c r="AB17" s="507" t="s">
         <v>40</v>
       </c>
-      <c r="AC17" s="476"/>
-      <c r="AD17" s="478" t="s">
+      <c r="AC17" s="509"/>
+      <c r="AD17" s="502" t="s">
         <v>58</v>
       </c>
-      <c r="AE17" s="478"/>
+      <c r="AE17" s="502"/>
       <c r="AF17" s="240" t="s">
         <v>103</v>
       </c>
-      <c r="AG17" s="477"/>
-      <c r="AH17" s="477"/>
-      <c r="AI17" s="477"/>
-      <c r="AJ17" s="477"/>
-      <c r="AK17" s="471"/>
-      <c r="AL17" s="471"/>
+      <c r="AG17" s="495"/>
+      <c r="AH17" s="495"/>
+      <c r="AI17" s="495"/>
+      <c r="AJ17" s="495"/>
+      <c r="AK17" s="504"/>
+      <c r="AL17" s="504"/>
       <c r="AN17" s="379"/>
     </row>
     <row r="18" spans="2:40" x14ac:dyDescent="0.25">
@@ -41550,14 +41538,14 @@
       <c r="Y32" s="41">
         <v>6.9971946482520506</v>
       </c>
-      <c r="AA32" s="472" t="s">
+      <c r="AA32" s="505" t="s">
         <v>25</v>
       </c>
-      <c r="AB32" s="472"/>
-      <c r="AC32" s="473" t="s">
+      <c r="AB32" s="505"/>
+      <c r="AC32" s="506" t="s">
         <v>40</v>
       </c>
-      <c r="AD32" s="473"/>
+      <c r="AD32" s="506"/>
       <c r="AI32" s="217" t="s">
         <v>76</v>
       </c>
@@ -43090,45 +43078,45 @@
       </c>
     </row>
     <row r="51" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="AA51" s="478" t="s">
+      <c r="AA51" s="502" t="s">
         <v>102</v>
       </c>
-      <c r="AB51" s="478"/>
-      <c r="AC51" s="478"/>
-      <c r="AD51" s="478"/>
-      <c r="AE51" s="478"/>
-      <c r="AF51" s="478"/>
-      <c r="AG51" s="478"/>
-      <c r="AH51" s="478"/>
-      <c r="AI51" s="478"/>
-      <c r="AJ51" s="478"/>
-      <c r="AK51" s="478"/>
-      <c r="AL51" s="478"/>
-      <c r="AM51" s="478"/>
-      <c r="AN51" s="478"/>
+      <c r="AB51" s="502"/>
+      <c r="AC51" s="502"/>
+      <c r="AD51" s="502"/>
+      <c r="AE51" s="502"/>
+      <c r="AF51" s="502"/>
+      <c r="AG51" s="502"/>
+      <c r="AH51" s="502"/>
+      <c r="AI51" s="502"/>
+      <c r="AJ51" s="502"/>
+      <c r="AK51" s="502"/>
+      <c r="AL51" s="502"/>
+      <c r="AM51" s="502"/>
+      <c r="AN51" s="502"/>
     </row>
     <row r="52" spans="2:40" x14ac:dyDescent="0.25">
       <c r="AA52" s="56"/>
-      <c r="AB52" s="489" t="s">
+      <c r="AB52" s="503" t="s">
         <v>72</v>
       </c>
-      <c r="AC52" s="489"/>
-      <c r="AD52" s="489"/>
-      <c r="AE52" s="489" t="s">
+      <c r="AC52" s="503"/>
+      <c r="AD52" s="503"/>
+      <c r="AE52" s="503" t="s">
         <v>73</v>
       </c>
-      <c r="AF52" s="489"/>
-      <c r="AG52" s="489"/>
-      <c r="AH52" s="489" t="s">
+      <c r="AF52" s="503"/>
+      <c r="AG52" s="503"/>
+      <c r="AH52" s="503" t="s">
         <v>74</v>
       </c>
-      <c r="AI52" s="489"/>
-      <c r="AJ52" s="489"/>
-      <c r="AK52" s="489" t="s">
+      <c r="AI52" s="503"/>
+      <c r="AJ52" s="503"/>
+      <c r="AK52" s="503" t="s">
         <v>75</v>
       </c>
-      <c r="AL52" s="489"/>
-      <c r="AM52" s="489"/>
+      <c r="AL52" s="503"/>
+      <c r="AM52" s="503"/>
       <c r="AN52" s="56"/>
     </row>
     <row r="53" spans="2:40" x14ac:dyDescent="0.25">
@@ -43223,34 +43211,34 @@
       </c>
     </row>
     <row r="55" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B55" s="486" t="s">
+      <c r="B55" s="499" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="487"/>
-      <c r="D55" s="487"/>
-      <c r="E55" s="487"/>
-      <c r="F55" s="488"/>
-      <c r="G55" s="486" t="s">
+      <c r="C55" s="500"/>
+      <c r="D55" s="500"/>
+      <c r="E55" s="500"/>
+      <c r="F55" s="501"/>
+      <c r="G55" s="499" t="s">
         <v>2</v>
       </c>
-      <c r="H55" s="487"/>
-      <c r="I55" s="487"/>
-      <c r="J55" s="487"/>
-      <c r="K55" s="488"/>
-      <c r="L55" s="486" t="s">
+      <c r="H55" s="500"/>
+      <c r="I55" s="500"/>
+      <c r="J55" s="500"/>
+      <c r="K55" s="501"/>
+      <c r="L55" s="499" t="s">
         <v>3</v>
       </c>
-      <c r="M55" s="487"/>
-      <c r="N55" s="487"/>
-      <c r="O55" s="487"/>
-      <c r="P55" s="488"/>
-      <c r="Q55" s="486" t="s">
+      <c r="M55" s="500"/>
+      <c r="N55" s="500"/>
+      <c r="O55" s="500"/>
+      <c r="P55" s="501"/>
+      <c r="Q55" s="499" t="s">
         <v>4</v>
       </c>
-      <c r="R55" s="487"/>
-      <c r="S55" s="487"/>
-      <c r="T55" s="487"/>
-      <c r="U55" s="488"/>
+      <c r="R55" s="500"/>
+      <c r="S55" s="500"/>
+      <c r="T55" s="500"/>
+      <c r="U55" s="501"/>
       <c r="AA55" s="206" t="s">
         <v>80</v>
       </c>
@@ -44461,20 +44449,20 @@
     </row>
     <row r="69" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B70" s="480" t="s">
+      <c r="B70" s="471" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="481"/>
-      <c r="D70" s="481"/>
-      <c r="E70" s="481"/>
-      <c r="F70" s="482"/>
-      <c r="G70" s="480" t="s">
+      <c r="C70" s="472"/>
+      <c r="D70" s="472"/>
+      <c r="E70" s="472"/>
+      <c r="F70" s="473"/>
+      <c r="G70" s="471" t="s">
         <v>6</v>
       </c>
-      <c r="H70" s="481"/>
-      <c r="I70" s="481"/>
-      <c r="J70" s="481"/>
-      <c r="K70" s="482"/>
+      <c r="H70" s="472"/>
+      <c r="I70" s="472"/>
+      <c r="J70" s="472"/>
+      <c r="K70" s="473"/>
     </row>
     <row r="71" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="146" t="s">
@@ -44882,20 +44870,20 @@
     </row>
     <row r="84" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B85" s="483" t="s">
+      <c r="B85" s="496" t="s">
         <v>7</v>
       </c>
-      <c r="C85" s="484"/>
-      <c r="D85" s="484"/>
-      <c r="E85" s="484"/>
-      <c r="F85" s="485"/>
-      <c r="G85" s="483" t="s">
+      <c r="C85" s="497"/>
+      <c r="D85" s="497"/>
+      <c r="E85" s="497"/>
+      <c r="F85" s="498"/>
+      <c r="G85" s="496" t="s">
         <v>8</v>
       </c>
-      <c r="H85" s="484"/>
-      <c r="I85" s="484"/>
-      <c r="J85" s="484"/>
-      <c r="K85" s="485"/>
+      <c r="H85" s="497"/>
+      <c r="I85" s="497"/>
+      <c r="J85" s="497"/>
+      <c r="K85" s="498"/>
     </row>
     <row r="86" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="161" t="s">
@@ -45305,34 +45293,34 @@
     </row>
     <row r="99" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="100" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B100" s="490" t="s">
+      <c r="B100" s="483" t="s">
         <v>9</v>
       </c>
-      <c r="C100" s="491"/>
-      <c r="D100" s="491"/>
-      <c r="E100" s="491"/>
-      <c r="F100" s="492"/>
-      <c r="G100" s="490" t="s">
+      <c r="C100" s="484"/>
+      <c r="D100" s="484"/>
+      <c r="E100" s="484"/>
+      <c r="F100" s="485"/>
+      <c r="G100" s="483" t="s">
         <v>10</v>
       </c>
-      <c r="H100" s="491"/>
-      <c r="I100" s="491"/>
-      <c r="J100" s="491"/>
-      <c r="K100" s="492"/>
-      <c r="L100" s="493" t="s">
+      <c r="H100" s="484"/>
+      <c r="I100" s="484"/>
+      <c r="J100" s="484"/>
+      <c r="K100" s="485"/>
+      <c r="L100" s="486" t="s">
         <v>11</v>
       </c>
-      <c r="M100" s="494"/>
-      <c r="N100" s="494"/>
-      <c r="O100" s="494"/>
-      <c r="P100" s="495"/>
-      <c r="Q100" s="490" t="s">
+      <c r="M100" s="487"/>
+      <c r="N100" s="487"/>
+      <c r="O100" s="487"/>
+      <c r="P100" s="488"/>
+      <c r="Q100" s="483" t="s">
         <v>12</v>
       </c>
-      <c r="R100" s="491"/>
-      <c r="S100" s="491"/>
-      <c r="T100" s="491"/>
-      <c r="U100" s="492"/>
+      <c r="R100" s="484"/>
+      <c r="S100" s="484"/>
+      <c r="T100" s="484"/>
+      <c r="U100" s="485"/>
     </row>
     <row r="101" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="171" t="s">
@@ -46120,34 +46108,34 @@
     </row>
     <row r="114" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="115" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B115" s="496" t="s">
+      <c r="B115" s="489" t="s">
         <v>13</v>
       </c>
-      <c r="C115" s="497"/>
-      <c r="D115" s="497"/>
-      <c r="E115" s="497"/>
-      <c r="F115" s="498"/>
-      <c r="G115" s="496" t="s">
+      <c r="C115" s="490"/>
+      <c r="D115" s="490"/>
+      <c r="E115" s="490"/>
+      <c r="F115" s="491"/>
+      <c r="G115" s="489" t="s">
         <v>14</v>
       </c>
-      <c r="H115" s="497"/>
-      <c r="I115" s="497"/>
-      <c r="J115" s="497"/>
-      <c r="K115" s="498"/>
-      <c r="L115" s="499" t="s">
+      <c r="H115" s="490"/>
+      <c r="I115" s="490"/>
+      <c r="J115" s="490"/>
+      <c r="K115" s="491"/>
+      <c r="L115" s="492" t="s">
         <v>15</v>
       </c>
-      <c r="M115" s="500"/>
-      <c r="N115" s="500"/>
-      <c r="O115" s="500"/>
-      <c r="P115" s="501"/>
-      <c r="Q115" s="496" t="s">
+      <c r="M115" s="493"/>
+      <c r="N115" s="493"/>
+      <c r="O115" s="493"/>
+      <c r="P115" s="494"/>
+      <c r="Q115" s="489" t="s">
         <v>16</v>
       </c>
-      <c r="R115" s="497"/>
-      <c r="S115" s="497"/>
-      <c r="T115" s="497"/>
-      <c r="U115" s="498"/>
+      <c r="R115" s="490"/>
+      <c r="S115" s="490"/>
+      <c r="T115" s="490"/>
+      <c r="U115" s="491"/>
     </row>
     <row r="116" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="181" t="s">
@@ -46935,34 +46923,34 @@
     </row>
     <row r="129" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="130" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B130" s="480" t="s">
+      <c r="B130" s="471" t="s">
         <v>17</v>
       </c>
-      <c r="C130" s="481"/>
-      <c r="D130" s="481"/>
-      <c r="E130" s="481"/>
-      <c r="F130" s="482"/>
-      <c r="G130" s="480" t="s">
+      <c r="C130" s="472"/>
+      <c r="D130" s="472"/>
+      <c r="E130" s="472"/>
+      <c r="F130" s="473"/>
+      <c r="G130" s="471" t="s">
         <v>18</v>
       </c>
-      <c r="H130" s="481"/>
-      <c r="I130" s="481"/>
-      <c r="J130" s="481"/>
-      <c r="K130" s="482"/>
-      <c r="L130" s="502" t="s">
+      <c r="H130" s="472"/>
+      <c r="I130" s="472"/>
+      <c r="J130" s="472"/>
+      <c r="K130" s="473"/>
+      <c r="L130" s="474" t="s">
         <v>19</v>
       </c>
-      <c r="M130" s="503"/>
-      <c r="N130" s="503"/>
-      <c r="O130" s="503"/>
-      <c r="P130" s="504"/>
-      <c r="Q130" s="480" t="s">
+      <c r="M130" s="475"/>
+      <c r="N130" s="475"/>
+      <c r="O130" s="475"/>
+      <c r="P130" s="476"/>
+      <c r="Q130" s="471" t="s">
         <v>20</v>
       </c>
-      <c r="R130" s="481"/>
-      <c r="S130" s="481"/>
-      <c r="T130" s="481"/>
-      <c r="U130" s="482"/>
+      <c r="R130" s="472"/>
+      <c r="S130" s="472"/>
+      <c r="T130" s="472"/>
+      <c r="U130" s="473"/>
     </row>
     <row r="131" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" s="146" t="s">
@@ -47750,27 +47738,27 @@
     </row>
     <row r="144" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="145" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B145" s="505" t="s">
+      <c r="B145" s="477" t="s">
         <v>21</v>
       </c>
-      <c r="C145" s="506"/>
-      <c r="D145" s="506"/>
-      <c r="E145" s="506"/>
-      <c r="F145" s="507"/>
-      <c r="G145" s="505" t="s">
+      <c r="C145" s="478"/>
+      <c r="D145" s="478"/>
+      <c r="E145" s="478"/>
+      <c r="F145" s="479"/>
+      <c r="G145" s="477" t="s">
         <v>22</v>
       </c>
-      <c r="H145" s="506"/>
-      <c r="I145" s="506"/>
-      <c r="J145" s="506"/>
-      <c r="K145" s="507"/>
-      <c r="L145" s="508" t="s">
+      <c r="H145" s="478"/>
+      <c r="I145" s="478"/>
+      <c r="J145" s="478"/>
+      <c r="K145" s="479"/>
+      <c r="L145" s="480" t="s">
         <v>23</v>
       </c>
-      <c r="M145" s="509"/>
-      <c r="N145" s="509"/>
-      <c r="O145" s="509"/>
-      <c r="P145" s="510"/>
+      <c r="M145" s="481"/>
+      <c r="N145" s="481"/>
+      <c r="O145" s="481"/>
+      <c r="P145" s="482"/>
     </row>
     <row r="146" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B146" s="191" t="s">
@@ -48369,36 +48357,6 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="G130:K130"/>
-    <mergeCell ref="L130:P130"/>
-    <mergeCell ref="Q130:U130"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="G145:K145"/>
-    <mergeCell ref="L145:P145"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="G100:K100"/>
-    <mergeCell ref="L100:P100"/>
-    <mergeCell ref="Q100:U100"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="G115:K115"/>
-    <mergeCell ref="L115:P115"/>
-    <mergeCell ref="Q115:U115"/>
-    <mergeCell ref="AH16:AH17"/>
-    <mergeCell ref="AI16:AI17"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="G70:K70"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="G85:K85"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="G55:K55"/>
-    <mergeCell ref="L55:P55"/>
-    <mergeCell ref="Q55:U55"/>
-    <mergeCell ref="AA51:AN51"/>
-    <mergeCell ref="AB52:AD52"/>
-    <mergeCell ref="AE52:AG52"/>
-    <mergeCell ref="AH52:AJ52"/>
-    <mergeCell ref="AK52:AM52"/>
     <mergeCell ref="AL1:AL2"/>
     <mergeCell ref="AL16:AL17"/>
     <mergeCell ref="AK16:AK17"/>
@@ -48415,6 +48373,36 @@
     <mergeCell ref="AH1:AH2"/>
     <mergeCell ref="AI1:AI2"/>
     <mergeCell ref="AG16:AG17"/>
+    <mergeCell ref="AH16:AH17"/>
+    <mergeCell ref="AI16:AI17"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="G70:K70"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="G85:K85"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="G55:K55"/>
+    <mergeCell ref="L55:P55"/>
+    <mergeCell ref="Q55:U55"/>
+    <mergeCell ref="AA51:AN51"/>
+    <mergeCell ref="AB52:AD52"/>
+    <mergeCell ref="AE52:AG52"/>
+    <mergeCell ref="AH52:AJ52"/>
+    <mergeCell ref="AK52:AM52"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="G100:K100"/>
+    <mergeCell ref="L100:P100"/>
+    <mergeCell ref="Q100:U100"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="G115:K115"/>
+    <mergeCell ref="L115:P115"/>
+    <mergeCell ref="Q115:U115"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="G130:K130"/>
+    <mergeCell ref="L130:P130"/>
+    <mergeCell ref="Q130:U130"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="G145:K145"/>
+    <mergeCell ref="L145:P145"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -48450,22 +48438,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="AG1" s="477" t="s">
+      <c r="AG1" s="495" t="s">
         <v>113</v>
       </c>
-      <c r="AH1" s="477" t="s">
+      <c r="AH1" s="495" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" s="477" t="s">
+      <c r="AI1" s="495" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="477" t="s">
+      <c r="AJ1" s="495" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="477" t="s">
+      <c r="AK1" s="495" t="s">
         <v>57</v>
       </c>
-      <c r="AL1" s="477" t="s">
+      <c r="AL1" s="495" t="s">
         <v>52</v>
       </c>
     </row>
@@ -48542,23 +48530,23 @@
       <c r="Y2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AB2" s="474" t="s">
+      <c r="AB2" s="507" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="475"/>
-      <c r="AD2" s="478" t="s">
+      <c r="AC2" s="508"/>
+      <c r="AD2" s="502" t="s">
         <v>58</v>
       </c>
-      <c r="AE2" s="478"/>
+      <c r="AE2" s="502"/>
       <c r="AF2" s="95" t="s">
         <v>103</v>
       </c>
-      <c r="AG2" s="477"/>
-      <c r="AH2" s="477"/>
-      <c r="AI2" s="477"/>
-      <c r="AJ2" s="477"/>
-      <c r="AK2" s="477"/>
-      <c r="AL2" s="477"/>
+      <c r="AG2" s="495"/>
+      <c r="AH2" s="495"/>
+      <c r="AI2" s="495"/>
+      <c r="AJ2" s="495"/>
+      <c r="AK2" s="495"/>
+      <c r="AL2" s="495"/>
     </row>
     <row r="3" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B3" s="14">
@@ -50099,22 +50087,22 @@
       <c r="Y15" s="315">
         <v>1.0235026535253984</v>
       </c>
-      <c r="AG15" s="477" t="s">
+      <c r="AG15" s="495" t="s">
         <v>56</v>
       </c>
-      <c r="AH15" s="477" t="s">
+      <c r="AH15" s="495" t="s">
         <v>57</v>
       </c>
-      <c r="AI15" s="477" t="s">
+      <c r="AI15" s="495" t="s">
         <v>52</v>
       </c>
-      <c r="AJ15" s="477" t="s">
+      <c r="AJ15" s="495" t="s">
         <v>56</v>
       </c>
-      <c r="AK15" s="477" t="s">
+      <c r="AK15" s="495" t="s">
         <v>57</v>
       </c>
-      <c r="AL15" s="477" t="s">
+      <c r="AL15" s="495" t="s">
         <v>52</v>
       </c>
       <c r="AM15" s="381"/>
@@ -50191,23 +50179,23 @@
       <c r="Y16" s="315">
         <v>1.0708870356330553</v>
       </c>
-      <c r="AB16" s="474" t="s">
+      <c r="AB16" s="507" t="s">
         <v>40</v>
       </c>
-      <c r="AC16" s="476"/>
-      <c r="AD16" s="478" t="s">
+      <c r="AC16" s="509"/>
+      <c r="AD16" s="502" t="s">
         <v>58</v>
       </c>
-      <c r="AE16" s="478"/>
+      <c r="AE16" s="502"/>
       <c r="AF16" s="95" t="s">
         <v>103</v>
       </c>
-      <c r="AG16" s="477"/>
-      <c r="AH16" s="477"/>
-      <c r="AI16" s="477"/>
-      <c r="AJ16" s="477"/>
-      <c r="AK16" s="477"/>
-      <c r="AL16" s="477"/>
+      <c r="AG16" s="495"/>
+      <c r="AH16" s="495"/>
+      <c r="AI16" s="495"/>
+      <c r="AJ16" s="495"/>
+      <c r="AK16" s="495"/>
+      <c r="AL16" s="495"/>
       <c r="AM16" s="381"/>
       <c r="AN16" s="381"/>
     </row>
@@ -51888,14 +51876,14 @@
       <c r="Y31" s="315">
         <v>6.6148597422289619</v>
       </c>
-      <c r="AA31" s="472" t="s">
+      <c r="AA31" s="505" t="s">
         <v>25</v>
       </c>
-      <c r="AB31" s="472"/>
-      <c r="AC31" s="473" t="s">
+      <c r="AB31" s="505"/>
+      <c r="AC31" s="506" t="s">
         <v>40</v>
       </c>
-      <c r="AD31" s="473"/>
+      <c r="AD31" s="506"/>
       <c r="AJ31" s="217" t="s">
         <v>76</v>
       </c>
@@ -54276,20 +54264,20 @@
       </c>
     </row>
     <row r="70" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="502" t="s">
+      <c r="B70" s="474" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="503"/>
-      <c r="D70" s="503"/>
-      <c r="E70" s="503"/>
-      <c r="F70" s="504"/>
-      <c r="G70" s="502" t="s">
+      <c r="C70" s="475"/>
+      <c r="D70" s="475"/>
+      <c r="E70" s="475"/>
+      <c r="F70" s="476"/>
+      <c r="G70" s="474" t="s">
         <v>6</v>
       </c>
-      <c r="H70" s="503"/>
-      <c r="I70" s="503"/>
-      <c r="J70" s="503"/>
-      <c r="K70" s="504"/>
+      <c r="H70" s="475"/>
+      <c r="I70" s="475"/>
+      <c r="J70" s="475"/>
+      <c r="K70" s="476"/>
       <c r="R70" s="388" t="s">
         <v>111</v>
       </c>
@@ -55584,34 +55572,34 @@
     </row>
     <row r="99" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="100" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B100" s="493" t="s">
+      <c r="B100" s="486" t="s">
         <v>9</v>
       </c>
-      <c r="C100" s="494"/>
-      <c r="D100" s="494"/>
-      <c r="E100" s="494"/>
-      <c r="F100" s="495"/>
-      <c r="G100" s="493" t="s">
+      <c r="C100" s="487"/>
+      <c r="D100" s="487"/>
+      <c r="E100" s="487"/>
+      <c r="F100" s="488"/>
+      <c r="G100" s="486" t="s">
         <v>10</v>
       </c>
-      <c r="H100" s="494"/>
-      <c r="I100" s="494"/>
-      <c r="J100" s="494"/>
-      <c r="K100" s="495"/>
-      <c r="L100" s="493" t="s">
+      <c r="H100" s="487"/>
+      <c r="I100" s="487"/>
+      <c r="J100" s="487"/>
+      <c r="K100" s="488"/>
+      <c r="L100" s="486" t="s">
         <v>11</v>
       </c>
-      <c r="M100" s="494"/>
-      <c r="N100" s="494"/>
-      <c r="O100" s="494"/>
-      <c r="P100" s="495"/>
-      <c r="Q100" s="493" t="s">
+      <c r="M100" s="487"/>
+      <c r="N100" s="487"/>
+      <c r="O100" s="487"/>
+      <c r="P100" s="488"/>
+      <c r="Q100" s="486" t="s">
         <v>12</v>
       </c>
-      <c r="R100" s="494"/>
-      <c r="S100" s="494"/>
-      <c r="T100" s="494"/>
-      <c r="U100" s="495"/>
+      <c r="R100" s="487"/>
+      <c r="S100" s="487"/>
+      <c r="T100" s="487"/>
+      <c r="U100" s="488"/>
     </row>
     <row r="101" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="171" t="s">
@@ -56399,34 +56387,34 @@
     </row>
     <row r="114" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="115" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B115" s="496" t="s">
+      <c r="B115" s="489" t="s">
         <v>13</v>
       </c>
-      <c r="C115" s="497"/>
-      <c r="D115" s="497"/>
-      <c r="E115" s="497"/>
-      <c r="F115" s="498"/>
-      <c r="G115" s="499" t="s">
+      <c r="C115" s="490"/>
+      <c r="D115" s="490"/>
+      <c r="E115" s="490"/>
+      <c r="F115" s="491"/>
+      <c r="G115" s="492" t="s">
         <v>14</v>
       </c>
-      <c r="H115" s="500"/>
-      <c r="I115" s="500"/>
-      <c r="J115" s="500"/>
-      <c r="K115" s="501"/>
-      <c r="L115" s="499" t="s">
+      <c r="H115" s="493"/>
+      <c r="I115" s="493"/>
+      <c r="J115" s="493"/>
+      <c r="K115" s="494"/>
+      <c r="L115" s="492" t="s">
         <v>15</v>
       </c>
-      <c r="M115" s="500"/>
-      <c r="N115" s="500"/>
-      <c r="O115" s="500"/>
-      <c r="P115" s="501"/>
-      <c r="Q115" s="499" t="s">
+      <c r="M115" s="493"/>
+      <c r="N115" s="493"/>
+      <c r="O115" s="493"/>
+      <c r="P115" s="494"/>
+      <c r="Q115" s="492" t="s">
         <v>16</v>
       </c>
-      <c r="R115" s="500"/>
-      <c r="S115" s="500"/>
-      <c r="T115" s="500"/>
-      <c r="U115" s="501"/>
+      <c r="R115" s="493"/>
+      <c r="S115" s="493"/>
+      <c r="T115" s="493"/>
+      <c r="U115" s="494"/>
     </row>
     <row r="116" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="181" t="s">
@@ -57098,34 +57086,34 @@
     </row>
     <row r="129" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="130" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B130" s="502" t="s">
+      <c r="B130" s="474" t="s">
         <v>17</v>
       </c>
-      <c r="C130" s="503"/>
-      <c r="D130" s="503"/>
-      <c r="E130" s="503"/>
-      <c r="F130" s="504"/>
-      <c r="G130" s="502" t="s">
+      <c r="C130" s="475"/>
+      <c r="D130" s="475"/>
+      <c r="E130" s="475"/>
+      <c r="F130" s="476"/>
+      <c r="G130" s="474" t="s">
         <v>18</v>
       </c>
-      <c r="H130" s="503"/>
-      <c r="I130" s="503"/>
-      <c r="J130" s="503"/>
-      <c r="K130" s="504"/>
-      <c r="L130" s="502" t="s">
+      <c r="H130" s="475"/>
+      <c r="I130" s="475"/>
+      <c r="J130" s="475"/>
+      <c r="K130" s="476"/>
+      <c r="L130" s="474" t="s">
         <v>19</v>
       </c>
-      <c r="M130" s="503"/>
-      <c r="N130" s="503"/>
-      <c r="O130" s="503"/>
-      <c r="P130" s="504"/>
-      <c r="Q130" s="502" t="s">
+      <c r="M130" s="475"/>
+      <c r="N130" s="475"/>
+      <c r="O130" s="475"/>
+      <c r="P130" s="476"/>
+      <c r="Q130" s="474" t="s">
         <v>20</v>
       </c>
-      <c r="R130" s="503"/>
-      <c r="S130" s="503"/>
-      <c r="T130" s="503"/>
-      <c r="U130" s="504"/>
+      <c r="R130" s="475"/>
+      <c r="S130" s="475"/>
+      <c r="T130" s="475"/>
+      <c r="U130" s="476"/>
     </row>
     <row r="131" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" s="146" t="s">
@@ -57913,27 +57901,27 @@
     </row>
     <row r="144" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="145" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B145" s="508" t="s">
+      <c r="B145" s="480" t="s">
         <v>21</v>
       </c>
-      <c r="C145" s="509"/>
-      <c r="D145" s="509"/>
-      <c r="E145" s="509"/>
-      <c r="F145" s="510"/>
-      <c r="G145" s="508" t="s">
+      <c r="C145" s="481"/>
+      <c r="D145" s="481"/>
+      <c r="E145" s="481"/>
+      <c r="F145" s="482"/>
+      <c r="G145" s="480" t="s">
         <v>22</v>
       </c>
-      <c r="H145" s="509"/>
-      <c r="I145" s="509"/>
-      <c r="J145" s="509"/>
-      <c r="K145" s="510"/>
-      <c r="L145" s="508" t="s">
+      <c r="H145" s="481"/>
+      <c r="I145" s="481"/>
+      <c r="J145" s="481"/>
+      <c r="K145" s="482"/>
+      <c r="L145" s="480" t="s">
         <v>23</v>
       </c>
-      <c r="M145" s="509"/>
-      <c r="N145" s="509"/>
-      <c r="O145" s="509"/>
-      <c r="P145" s="510"/>
+      <c r="M145" s="481"/>
+      <c r="N145" s="481"/>
+      <c r="O145" s="481"/>
+      <c r="P145" s="482"/>
     </row>
     <row r="146" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B146" s="191" t="s">
@@ -58532,17 +58520,24 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="G145:K145"/>
-    <mergeCell ref="L145:P145"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="G115:K115"/>
-    <mergeCell ref="L115:P115"/>
-    <mergeCell ref="Q115:U115"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="G130:K130"/>
-    <mergeCell ref="L130:P130"/>
-    <mergeCell ref="Q130:U130"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="AK15:AK16"/>
+    <mergeCell ref="AL15:AL16"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AD16:AE16"/>
+    <mergeCell ref="AA31:AB31"/>
+    <mergeCell ref="AC31:AD31"/>
+    <mergeCell ref="AJ15:AJ16"/>
+    <mergeCell ref="AG15:AG16"/>
+    <mergeCell ref="AH15:AH16"/>
+    <mergeCell ref="AI15:AI16"/>
     <mergeCell ref="Q100:U100"/>
     <mergeCell ref="B55:F55"/>
     <mergeCell ref="G55:K55"/>
@@ -58555,24 +58550,17 @@
     <mergeCell ref="B100:F100"/>
     <mergeCell ref="G100:K100"/>
     <mergeCell ref="L100:P100"/>
-    <mergeCell ref="AK15:AK16"/>
-    <mergeCell ref="AL15:AL16"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AD16:AE16"/>
-    <mergeCell ref="AA31:AB31"/>
-    <mergeCell ref="AC31:AD31"/>
-    <mergeCell ref="AJ15:AJ16"/>
-    <mergeCell ref="AG15:AG16"/>
-    <mergeCell ref="AH15:AH16"/>
-    <mergeCell ref="AI15:AI16"/>
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="AH1:AH2"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="Q115:U115"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="G130:K130"/>
+    <mergeCell ref="L130:P130"/>
+    <mergeCell ref="Q130:U130"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="G145:K145"/>
+    <mergeCell ref="L145:P145"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="G115:K115"/>
+    <mergeCell ref="L115:P115"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -58584,8 +58572,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView topLeftCell="I9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView topLeftCell="AB1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58606,22 +58594,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="478" t="s">
+      <c r="A1" s="502" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="521"/>
-      <c r="C1" s="521"/>
-      <c r="D1" s="521"/>
-      <c r="E1" s="521"/>
-      <c r="F1" s="521"/>
-      <c r="G1" s="521"/>
-      <c r="H1" s="521"/>
-      <c r="I1" s="521"/>
-      <c r="J1" s="521"/>
-      <c r="K1" s="521"/>
-      <c r="L1" s="521"/>
-      <c r="M1" s="521"/>
-      <c r="N1" s="478"/>
+      <c r="B1" s="517"/>
+      <c r="C1" s="517"/>
+      <c r="D1" s="517"/>
+      <c r="E1" s="517"/>
+      <c r="F1" s="517"/>
+      <c r="G1" s="517"/>
+      <c r="H1" s="517"/>
+      <c r="I1" s="517"/>
+      <c r="J1" s="517"/>
+      <c r="K1" s="517"/>
+      <c r="L1" s="517"/>
+      <c r="M1" s="517"/>
+      <c r="N1" s="502"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="216"/>
@@ -58646,11 +58634,11 @@
       <c r="L2" s="519"/>
       <c r="M2" s="520"/>
       <c r="N2" s="232"/>
-      <c r="O2" s="517" t="s">
+      <c r="O2" s="521" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="517"/>
-      <c r="Q2" s="517"/>
+      <c r="P2" s="521"/>
+      <c r="Q2" s="521"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="217" t="s">
@@ -59426,22 +59414,22 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="478" t="s">
+      <c r="A16" s="502" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="521"/>
-      <c r="C16" s="521"/>
-      <c r="D16" s="521"/>
-      <c r="E16" s="521"/>
-      <c r="F16" s="521"/>
-      <c r="G16" s="521"/>
-      <c r="H16" s="521"/>
-      <c r="I16" s="521"/>
-      <c r="J16" s="521"/>
-      <c r="K16" s="521"/>
-      <c r="L16" s="521"/>
-      <c r="M16" s="521"/>
-      <c r="N16" s="478"/>
+      <c r="B16" s="517"/>
+      <c r="C16" s="517"/>
+      <c r="D16" s="517"/>
+      <c r="E16" s="517"/>
+      <c r="F16" s="517"/>
+      <c r="G16" s="517"/>
+      <c r="H16" s="517"/>
+      <c r="I16" s="517"/>
+      <c r="J16" s="517"/>
+      <c r="K16" s="517"/>
+      <c r="L16" s="517"/>
+      <c r="M16" s="517"/>
+      <c r="N16" s="502"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="216"/>
@@ -59466,11 +59454,11 @@
       <c r="L17" s="519"/>
       <c r="M17" s="520"/>
       <c r="N17" s="232"/>
-      <c r="O17" s="517" t="s">
+      <c r="O17" s="521" t="s">
         <v>27</v>
       </c>
-      <c r="P17" s="517"/>
-      <c r="Q17" s="517"/>
+      <c r="P17" s="521"/>
+      <c r="Q17" s="521"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="217" t="s">
@@ -59707,9 +59695,7 @@
         <f t="shared" si="7"/>
         <v>0.25528328492852753</v>
       </c>
-      <c r="N21" s="366">
-        <v>-0.32001589401318498</v>
-      </c>
+      <c r="N21" s="366"/>
       <c r="O21" s="466">
         <v>-0.32588985777528645</v>
       </c>
@@ -60111,22 +60097,22 @@
       </c>
     </row>
     <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="478" t="s">
+      <c r="A29" s="502" t="s">
         <v>106</v>
       </c>
-      <c r="B29" s="521"/>
-      <c r="C29" s="521"/>
-      <c r="D29" s="521"/>
-      <c r="E29" s="521"/>
-      <c r="F29" s="521"/>
-      <c r="G29" s="521"/>
-      <c r="H29" s="521"/>
-      <c r="I29" s="521"/>
-      <c r="J29" s="521"/>
-      <c r="K29" s="521"/>
-      <c r="L29" s="521"/>
-      <c r="M29" s="521"/>
-      <c r="N29" s="478"/>
+      <c r="B29" s="517"/>
+      <c r="C29" s="517"/>
+      <c r="D29" s="517"/>
+      <c r="E29" s="517"/>
+      <c r="F29" s="517"/>
+      <c r="G29" s="517"/>
+      <c r="H29" s="517"/>
+      <c r="I29" s="517"/>
+      <c r="J29" s="517"/>
+      <c r="K29" s="517"/>
+      <c r="L29" s="517"/>
+      <c r="M29" s="517"/>
+      <c r="N29" s="502"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="216"/>
@@ -60153,11 +60139,11 @@
       <c r="N30" s="232" t="s">
         <v>119</v>
       </c>
-      <c r="O30" s="517" t="s">
+      <c r="O30" s="521" t="s">
         <v>27</v>
       </c>
-      <c r="P30" s="517"/>
-      <c r="Q30" s="517"/>
+      <c r="P30" s="521"/>
+      <c r="Q30" s="521"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="217" t="s">
@@ -60734,11 +60720,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
     <mergeCell ref="O2:Q2"/>
     <mergeCell ref="O17:Q17"/>
     <mergeCell ref="O30:Q30"/>
@@ -60752,6 +60733,11 @@
     <mergeCell ref="E30:G30"/>
     <mergeCell ref="H30:J30"/>
     <mergeCell ref="K30:M30"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -60762,8 +60748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D740D4BE-AE48-479D-87CF-305597DEB593}">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AF23" sqref="AF23"/>
+    <sheetView tabSelected="1" topLeftCell="K15" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60783,22 +60769,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="478" t="s">
+      <c r="A1" s="502" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="521"/>
-      <c r="C1" s="521"/>
-      <c r="D1" s="521"/>
-      <c r="E1" s="521"/>
-      <c r="F1" s="521"/>
-      <c r="G1" s="521"/>
-      <c r="H1" s="521"/>
-      <c r="I1" s="521"/>
-      <c r="J1" s="521"/>
-      <c r="K1" s="521"/>
-      <c r="L1" s="521"/>
-      <c r="M1" s="521"/>
-      <c r="N1" s="478"/>
+      <c r="B1" s="517"/>
+      <c r="C1" s="517"/>
+      <c r="D1" s="517"/>
+      <c r="E1" s="517"/>
+      <c r="F1" s="517"/>
+      <c r="G1" s="517"/>
+      <c r="H1" s="517"/>
+      <c r="I1" s="517"/>
+      <c r="J1" s="517"/>
+      <c r="K1" s="517"/>
+      <c r="L1" s="517"/>
+      <c r="M1" s="517"/>
+      <c r="N1" s="502"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="216"/>
@@ -61531,22 +61517,22 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="478" t="s">
+      <c r="A16" s="502" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="521"/>
-      <c r="C16" s="521"/>
-      <c r="D16" s="521"/>
-      <c r="E16" s="521"/>
-      <c r="F16" s="521"/>
-      <c r="G16" s="521"/>
-      <c r="H16" s="521"/>
-      <c r="I16" s="521"/>
-      <c r="J16" s="521"/>
-      <c r="K16" s="521"/>
-      <c r="L16" s="521"/>
-      <c r="M16" s="521"/>
-      <c r="N16" s="478"/>
+      <c r="B16" s="517"/>
+      <c r="C16" s="517"/>
+      <c r="D16" s="517"/>
+      <c r="E16" s="517"/>
+      <c r="F16" s="517"/>
+      <c r="G16" s="517"/>
+      <c r="H16" s="517"/>
+      <c r="I16" s="517"/>
+      <c r="J16" s="517"/>
+      <c r="K16" s="517"/>
+      <c r="L16" s="517"/>
+      <c r="M16" s="517"/>
+      <c r="N16" s="502"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="216"/>
@@ -62156,22 +62142,22 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="478" t="s">
+      <c r="A29" s="502" t="s">
         <v>106</v>
       </c>
-      <c r="B29" s="521"/>
-      <c r="C29" s="521"/>
-      <c r="D29" s="521"/>
-      <c r="E29" s="521"/>
-      <c r="F29" s="521"/>
-      <c r="G29" s="521"/>
-      <c r="H29" s="521"/>
-      <c r="I29" s="521"/>
-      <c r="J29" s="521"/>
-      <c r="K29" s="521"/>
-      <c r="L29" s="521"/>
-      <c r="M29" s="521"/>
-      <c r="N29" s="478"/>
+      <c r="B29" s="517"/>
+      <c r="C29" s="517"/>
+      <c r="D29" s="517"/>
+      <c r="E29" s="517"/>
+      <c r="F29" s="517"/>
+      <c r="G29" s="517"/>
+      <c r="H29" s="517"/>
+      <c r="I29" s="517"/>
+      <c r="J29" s="517"/>
+      <c r="K29" s="517"/>
+      <c r="L29" s="517"/>
+      <c r="M29" s="517"/>
+      <c r="N29" s="502"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="216"/>
@@ -62723,21 +62709,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="A16:N16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:M17"/>
     <mergeCell ref="A29:N29"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="E30:G30"/>
     <mergeCell ref="H30:J30"/>
     <mergeCell ref="K30:M30"/>
-    <mergeCell ref="A16:N16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>